<commit_message>
fixed #24 TournRPG-24 敵を変化させる
</commit_message>
<xml_diff>
--- a/docs/enemy.xlsx
+++ b/docs/enemy.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="256">
   <si>
     <t>id</t>
   </si>
@@ -47,10 +47,739 @@
     <t>int</t>
   </si>
   <si>
+    <t>BAT</t>
+  </si>
+  <si>
+    <t>コウモリ</t>
+  </si>
+  <si>
+    <t>e001.png</t>
+  </si>
+  <si>
+    <t>BAT_2</t>
+  </si>
+  <si>
+    <t>レッドスライム</t>
+  </si>
+  <si>
+    <t>e001a.png</t>
+  </si>
+  <si>
+    <t>BAT_3</t>
+  </si>
+  <si>
+    <t>ゴールデンコウモリ</t>
+  </si>
+  <si>
+    <t>e001b.png</t>
+  </si>
+  <si>
+    <t>WOLF</t>
+  </si>
+  <si>
+    <t>オオカミ</t>
+  </si>
+  <si>
+    <t>e002.png</t>
+  </si>
+  <si>
+    <t>WOLF_2</t>
+  </si>
+  <si>
+    <t>ウルフ</t>
+  </si>
+  <si>
+    <t>e002a.png</t>
+  </si>
+  <si>
+    <t>WOLF_3</t>
+  </si>
+  <si>
+    <t>レッドウルフ</t>
+  </si>
+  <si>
+    <t>e002b.png</t>
+  </si>
+  <si>
+    <t>SNAKE</t>
+  </si>
+  <si>
+    <t>ヘビ</t>
+  </si>
+  <si>
+    <t>e003.png</t>
+  </si>
+  <si>
+    <t>SNAKE_2</t>
+  </si>
+  <si>
+    <t>毒蛇</t>
+  </si>
+  <si>
+    <t>e003a.png</t>
+  </si>
+  <si>
+    <t>SNAME_3</t>
+  </si>
+  <si>
+    <t>スネーク</t>
+  </si>
+  <si>
+    <t>e003b.png</t>
+  </si>
+  <si>
+    <t>BEETLE</t>
+  </si>
+  <si>
+    <t>ビートル</t>
+  </si>
+  <si>
+    <t>e004.png</t>
+  </si>
+  <si>
+    <t>BEETLE_2</t>
+  </si>
+  <si>
+    <t>バトルビートル</t>
+  </si>
+  <si>
+    <t>e004a.png</t>
+  </si>
+  <si>
+    <t>BEETLE_3</t>
+  </si>
+  <si>
+    <t>ゴールデンビートル</t>
+  </si>
+  <si>
+    <t>e004b.png</t>
+  </si>
+  <si>
+    <t>WORM</t>
+  </si>
+  <si>
+    <t>大ミミズ</t>
+  </si>
+  <si>
+    <t>e005.png</t>
+  </si>
+  <si>
+    <t>WORM_2</t>
+  </si>
+  <si>
+    <t>ワーム</t>
+  </si>
+  <si>
+    <t>e005a.png</t>
+  </si>
+  <si>
+    <t>WORM_3</t>
+  </si>
+  <si>
+    <t>アイアンワーム</t>
+  </si>
+  <si>
+    <t>e005b.png</t>
+  </si>
+  <si>
+    <t>WOOD</t>
+  </si>
+  <si>
+    <t>人面植物</t>
+  </si>
+  <si>
+    <t>e006.png</t>
+  </si>
+  <si>
+    <t>WOOD_2</t>
+  </si>
+  <si>
+    <t>ピンクマン</t>
+  </si>
+  <si>
+    <t>e006a.png</t>
+  </si>
+  <si>
+    <t>WOOD_3</t>
+  </si>
+  <si>
+    <t>ウッドマン</t>
+  </si>
+  <si>
+    <t>e006b.png</t>
+  </si>
+  <si>
+    <t>FLOWER</t>
+  </si>
+  <si>
+    <t>人面花</t>
+  </si>
+  <si>
+    <t>e007.png</t>
+  </si>
+  <si>
+    <t>FLOWER_2</t>
+  </si>
+  <si>
+    <t>おばけフラワー</t>
+  </si>
+  <si>
+    <t>e007a.png</t>
+  </si>
+  <si>
+    <t>FLOWER_3</t>
+  </si>
+  <si>
+    <t>フラワーマシーン</t>
+  </si>
+  <si>
+    <t>e007b.png</t>
+  </si>
+  <si>
+    <t>MASHROOM</t>
+  </si>
+  <si>
+    <t>きのこマン</t>
+  </si>
+  <si>
+    <t>e008.png</t>
+  </si>
+  <si>
+    <t>MASHROOM_2</t>
+  </si>
+  <si>
+    <t>きのこウーマン</t>
+  </si>
+  <si>
+    <t>e008a.png</t>
+  </si>
+  <si>
+    <t>MASHROOM_3</t>
+  </si>
+  <si>
+    <t>マッシュマン</t>
+  </si>
+  <si>
+    <t>e008b.png</t>
+  </si>
+  <si>
     <t>SLIME</t>
   </si>
   <si>
     <t>スライム</t>
+  </si>
+  <si>
+    <t>e009.png</t>
+  </si>
+  <si>
+    <t>SLIME_2</t>
+  </si>
+  <si>
+    <t>e009a.png</t>
+  </si>
+  <si>
+    <t>SLIME_3</t>
+  </si>
+  <si>
+    <t>鋼のスライム</t>
+  </si>
+  <si>
+    <t>e009b.png</t>
+  </si>
+  <si>
+    <t>GHOST</t>
+  </si>
+  <si>
+    <t>おばけ</t>
+  </si>
+  <si>
+    <t>e010.png</t>
+  </si>
+  <si>
+    <t>GHOST_2</t>
+  </si>
+  <si>
+    <t>ゴースト</t>
+  </si>
+  <si>
+    <t>e010a.png</t>
+  </si>
+  <si>
+    <t>GHOST_3</t>
+  </si>
+  <si>
+    <t>亡霊</t>
+  </si>
+  <si>
+    <t>e010b.png</t>
+  </si>
+  <si>
+    <t>ZOMB</t>
+  </si>
+  <si>
+    <t>ゾンビ</t>
+  </si>
+  <si>
+    <t>e011.png</t>
+  </si>
+  <si>
+    <t>ZOMB_2</t>
+  </si>
+  <si>
+    <t>動く死体</t>
+  </si>
+  <si>
+    <t>e011a.png</t>
+  </si>
+  <si>
+    <t>ZOMB_3</t>
+  </si>
+  <si>
+    <t>危険な死体</t>
+  </si>
+  <si>
+    <t>e011b.png</t>
+  </si>
+  <si>
+    <t>WISP</t>
+  </si>
+  <si>
+    <t>鬼火</t>
+  </si>
+  <si>
+    <t>e012.png</t>
+  </si>
+  <si>
+    <t>WISP_2</t>
+  </si>
+  <si>
+    <t>ウィルオウィスプ</t>
+  </si>
+  <si>
+    <t>e012a.png</t>
+  </si>
+  <si>
+    <t>WISP_3</t>
+  </si>
+  <si>
+    <t>邪悪な精霊</t>
+  </si>
+  <si>
+    <t>e012b.png</t>
+  </si>
+  <si>
+    <t>OAK</t>
+  </si>
+  <si>
+    <t>オーク</t>
+  </si>
+  <si>
+    <t>e013.png</t>
+  </si>
+  <si>
+    <t>OAK_2</t>
+  </si>
+  <si>
+    <t>オーク2</t>
+  </si>
+  <si>
+    <t>e013a.png</t>
+  </si>
+  <si>
+    <t>OAK_3</t>
+  </si>
+  <si>
+    <t>オーク3</t>
+  </si>
+  <si>
+    <t>e013b.png</t>
+  </si>
+  <si>
+    <t>WEREWOLF</t>
+  </si>
+  <si>
+    <t>狼小僧</t>
+  </si>
+  <si>
+    <t>e014.png</t>
+  </si>
+  <si>
+    <t>WEREWOLF_2</t>
+  </si>
+  <si>
+    <t>ワーウルフ</t>
+  </si>
+  <si>
+    <t>e014a.png</t>
+  </si>
+  <si>
+    <t>WEREWOLF_3</t>
+  </si>
+  <si>
+    <t>ワーウルフ２</t>
+  </si>
+  <si>
+    <t>e014b.png</t>
+  </si>
+  <si>
+    <t>TROLL</t>
+  </si>
+  <si>
+    <t>ゴブリン</t>
+  </si>
+  <si>
+    <t>e015.png</t>
+  </si>
+  <si>
+    <t>TROLL_2</t>
+  </si>
+  <si>
+    <t>ゴブリン2</t>
+  </si>
+  <si>
+    <t>e015a.png</t>
+  </si>
+  <si>
+    <t>TROLL_3</t>
+  </si>
+  <si>
+    <t>ゴブリン3</t>
+  </si>
+  <si>
+    <t>e015b.png</t>
+  </si>
+  <si>
+    <t>LIZARD</t>
+  </si>
+  <si>
+    <t>エリマキトカゲ</t>
+  </si>
+  <si>
+    <t>e016.png</t>
+  </si>
+  <si>
+    <t>LIZARD_2</t>
+  </si>
+  <si>
+    <t>エリマキトカゲ2</t>
+  </si>
+  <si>
+    <t>e016a.png</t>
+  </si>
+  <si>
+    <t>LIZARD_3</t>
+  </si>
+  <si>
+    <t>エリマキトカゲ3</t>
+  </si>
+  <si>
+    <t>e016b.png</t>
+  </si>
+  <si>
+    <t>WRAITH</t>
+  </si>
+  <si>
+    <t>悪霊</t>
+  </si>
+  <si>
+    <t>e017.png</t>
+  </si>
+  <si>
+    <t>WRAITH_2</t>
+  </si>
+  <si>
+    <t>レイス</t>
+  </si>
+  <si>
+    <t>e017a.png</t>
+  </si>
+  <si>
+    <t>WRAITH_3</t>
+  </si>
+  <si>
+    <t>死神</t>
+  </si>
+  <si>
+    <t>e017b.png</t>
+  </si>
+  <si>
+    <t>FIGHTER</t>
+  </si>
+  <si>
+    <t>剣士</t>
+  </si>
+  <si>
+    <t>e018.png</t>
+  </si>
+  <si>
+    <t>FIGHTER_2</t>
+  </si>
+  <si>
+    <t>ファイター</t>
+  </si>
+  <si>
+    <t>e018a.png</t>
+  </si>
+  <si>
+    <t>FIGHTER_3</t>
+  </si>
+  <si>
+    <t>悪魔剣士</t>
+  </si>
+  <si>
+    <t>e018b.png</t>
+  </si>
+  <si>
+    <t>OGRE</t>
+  </si>
+  <si>
+    <t>オニ</t>
+  </si>
+  <si>
+    <t>e019.png</t>
+  </si>
+  <si>
+    <t>OGRE_2</t>
+  </si>
+  <si>
+    <t>オーガ</t>
+  </si>
+  <si>
+    <t>e019a.png</t>
+  </si>
+  <si>
+    <t>OGRE_3</t>
+  </si>
+  <si>
+    <t>デスオーガ</t>
+  </si>
+  <si>
+    <t>e019b.png</t>
+  </si>
+  <si>
+    <t>MONOEYE</t>
+  </si>
+  <si>
+    <t>モノアイ</t>
+  </si>
+  <si>
+    <t>e020.png</t>
+  </si>
+  <si>
+    <t>MONOEYE_2</t>
+  </si>
+  <si>
+    <t>一つ目小僧</t>
+  </si>
+  <si>
+    <t>e020a.png</t>
+  </si>
+  <si>
+    <t>MONOEYE_3</t>
+  </si>
+  <si>
+    <t>人喰いオニ</t>
+  </si>
+  <si>
+    <t>e020b.png</t>
+  </si>
+  <si>
+    <t>DRAGON</t>
+  </si>
+  <si>
+    <t>ドラゴン</t>
+  </si>
+  <si>
+    <t>e021.png</t>
+  </si>
+  <si>
+    <t>DRAGON_2</t>
+  </si>
+  <si>
+    <t>レッドドラゴン</t>
+  </si>
+  <si>
+    <t>e021a.png</t>
+  </si>
+  <si>
+    <t>DRAGON_3</t>
+  </si>
+  <si>
+    <t>ダークドラゴン</t>
+  </si>
+  <si>
+    <t>e021b.png</t>
+  </si>
+  <si>
+    <t>GRIFFON</t>
+  </si>
+  <si>
+    <t>グリフォン</t>
+  </si>
+  <si>
+    <t>e022.png</t>
+  </si>
+  <si>
+    <t>GRIFFON_2</t>
+  </si>
+  <si>
+    <t>グリフィン</t>
+  </si>
+  <si>
+    <t>e022a.png</t>
+  </si>
+  <si>
+    <t>GRIFFON_3</t>
+  </si>
+  <si>
+    <t>グリュプス</t>
+  </si>
+  <si>
+    <t>e022b.png</t>
+  </si>
+  <si>
+    <t>CERBERUS</t>
+  </si>
+  <si>
+    <t>レッドケルベロス</t>
+  </si>
+  <si>
+    <t>e023.png</t>
+  </si>
+  <si>
+    <t>CERBERUS_2</t>
+  </si>
+  <si>
+    <t>地獄の番犬</t>
+  </si>
+  <si>
+    <t>e023a.png</t>
+  </si>
+  <si>
+    <t>CERBERUS_3</t>
+  </si>
+  <si>
+    <t>ケルベロス</t>
+  </si>
+  <si>
+    <t>e023b.png</t>
+  </si>
+  <si>
+    <t>DEMON</t>
+  </si>
+  <si>
+    <t>サタン</t>
+  </si>
+  <si>
+    <t>e024.png</t>
+  </si>
+  <si>
+    <t>DEMON_2</t>
+  </si>
+  <si>
+    <t>デビル</t>
+  </si>
+  <si>
+    <t>e024a.png</t>
+  </si>
+  <si>
+    <t>DEMON_3</t>
+  </si>
+  <si>
+    <t>デーモン</t>
+  </si>
+  <si>
+    <t>e024b.png</t>
+  </si>
+  <si>
+    <t>MAGICIAN</t>
+  </si>
+  <si>
+    <t>ネクロマンサー</t>
+  </si>
+  <si>
+    <t>e025.png</t>
+  </si>
+  <si>
+    <t>MAGICIAN_2</t>
+  </si>
+  <si>
+    <t>マジシャン</t>
+  </si>
+  <si>
+    <t>e025a.png</t>
+  </si>
+  <si>
+    <t>MAGICIAN_3</t>
+  </si>
+  <si>
+    <t>カースメーカー</t>
+  </si>
+  <si>
+    <t>e025b.png</t>
+  </si>
+  <si>
+    <t>KNIGHT</t>
+  </si>
+  <si>
+    <t>ナイト</t>
+  </si>
+  <si>
+    <t>e026.png</t>
+  </si>
+  <si>
+    <t>KNIGHT_2</t>
+  </si>
+  <si>
+    <t>レッドナイト</t>
+  </si>
+  <si>
+    <t>e026a.png</t>
+  </si>
+  <si>
+    <t>KNIGHT_3</t>
+  </si>
+  <si>
+    <t>ダークナイト</t>
+  </si>
+  <si>
+    <t>e026b.png</t>
+  </si>
+  <si>
+    <t>DEVIL_MINSTER</t>
+  </si>
+  <si>
+    <t>魔王の使者</t>
+  </si>
+  <si>
+    <t>e027.png</t>
+  </si>
+  <si>
+    <t>BIG_MAGICIAN</t>
+  </si>
+  <si>
+    <t>混沌の魔術師</t>
+  </si>
+  <si>
+    <t>e028.png</t>
+  </si>
+  <si>
+    <t>CHAOS</t>
+  </si>
+  <si>
+    <t>ケイオス</t>
+  </si>
+  <si>
+    <t>e029.png</t>
+  </si>
+  <si>
+    <t>DEVIL</t>
+  </si>
+  <si>
+    <t>魔王</t>
+  </si>
+  <si>
+    <t>e030.png</t>
   </si>
 </sst>
 </file>
@@ -1418,7 +2147,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J84"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="C3" xSplit="2" ySplit="2" activePane="bottomRight" state="frozenSplit"/>
@@ -1427,8 +2156,8 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.55" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="14.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.57031" style="1" customWidth="1"/>
-    <col min="3" max="3" width="5.61719" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5078" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.1484" style="1" customWidth="1"/>
     <col min="4" max="4" width="4.625" style="1" customWidth="1"/>
     <col min="5" max="5" width="4" style="1" customWidth="1"/>
     <col min="6" max="6" width="2.75" style="1" customWidth="1"/>
@@ -1479,7 +2208,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s" s="4">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s" s="4">
         <v>10</v>
@@ -1510,8 +2239,8 @@
       <c r="B3" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="C3" s="5">
-        <v>1</v>
+      <c r="C3" t="s" s="5">
+        <v>13</v>
       </c>
       <c r="D3" s="5">
         <v>25</v>
@@ -1520,18 +2249,2610 @@
         <v>3</v>
       </c>
       <c r="F3" s="6">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G3" s="6">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="H3" s="6">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="I3" s="6">
         <v>1</v>
       </c>
       <c r="J3" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" ht="20" customHeight="1">
+      <c r="A4" t="s" s="3">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s" s="4">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s" s="5">
+        <v>16</v>
+      </c>
+      <c r="D4" s="5">
+        <v>30</v>
+      </c>
+      <c r="E4" s="6">
+        <v>5</v>
+      </c>
+      <c r="F4" s="6">
+        <v>6</v>
+      </c>
+      <c r="G4" s="6">
+        <v>5</v>
+      </c>
+      <c r="H4" s="6">
+        <v>4</v>
+      </c>
+      <c r="I4" s="6">
+        <v>2</v>
+      </c>
+      <c r="J4" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" ht="20" customHeight="1">
+      <c r="A5" t="s" s="3">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s" s="4">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s" s="5">
+        <v>19</v>
+      </c>
+      <c r="D5" s="5">
+        <v>35</v>
+      </c>
+      <c r="E5" s="6">
+        <v>6</v>
+      </c>
+      <c r="F5" s="6">
+        <v>5</v>
+      </c>
+      <c r="G5" s="6">
+        <v>4</v>
+      </c>
+      <c r="H5" s="6">
+        <v>3</v>
+      </c>
+      <c r="I5" s="6">
+        <v>2</v>
+      </c>
+      <c r="J5" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" ht="20" customHeight="1">
+      <c r="A6" t="s" s="3">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s" s="4">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s" s="5">
+        <v>22</v>
+      </c>
+      <c r="D6" s="5">
+        <v>35</v>
+      </c>
+      <c r="E6" s="6">
+        <v>6</v>
+      </c>
+      <c r="F6" s="6">
+        <v>5</v>
+      </c>
+      <c r="G6" s="6">
+        <v>4</v>
+      </c>
+      <c r="H6" s="6">
+        <v>3</v>
+      </c>
+      <c r="I6" s="6">
+        <v>2</v>
+      </c>
+      <c r="J6" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" ht="20" customHeight="1">
+      <c r="A7" t="s" s="3">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s" s="4">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s" s="5">
+        <v>25</v>
+      </c>
+      <c r="D7" s="5">
+        <v>35</v>
+      </c>
+      <c r="E7" s="6">
+        <v>6</v>
+      </c>
+      <c r="F7" s="6">
+        <v>5</v>
+      </c>
+      <c r="G7" s="6">
+        <v>4</v>
+      </c>
+      <c r="H7" s="6">
+        <v>3</v>
+      </c>
+      <c r="I7" s="6">
+        <v>2</v>
+      </c>
+      <c r="J7" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" ht="20" customHeight="1">
+      <c r="A8" t="s" s="3">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s" s="4">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s" s="5">
+        <v>28</v>
+      </c>
+      <c r="D8" s="5">
+        <v>35</v>
+      </c>
+      <c r="E8" s="6">
+        <v>6</v>
+      </c>
+      <c r="F8" s="6">
+        <v>5</v>
+      </c>
+      <c r="G8" s="6">
+        <v>4</v>
+      </c>
+      <c r="H8" s="6">
+        <v>3</v>
+      </c>
+      <c r="I8" s="6">
+        <v>2</v>
+      </c>
+      <c r="J8" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" ht="20" customHeight="1">
+      <c r="A9" t="s" s="3">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s" s="4">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s" s="5">
+        <v>31</v>
+      </c>
+      <c r="D9" s="5">
+        <v>35</v>
+      </c>
+      <c r="E9" s="6">
+        <v>6</v>
+      </c>
+      <c r="F9" s="6">
+        <v>5</v>
+      </c>
+      <c r="G9" s="6">
+        <v>4</v>
+      </c>
+      <c r="H9" s="6">
+        <v>3</v>
+      </c>
+      <c r="I9" s="6">
+        <v>2</v>
+      </c>
+      <c r="J9" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" ht="20" customHeight="1">
+      <c r="A10" t="s" s="3">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s" s="4">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s" s="5">
+        <v>34</v>
+      </c>
+      <c r="D10" s="5">
+        <v>35</v>
+      </c>
+      <c r="E10" s="6">
+        <v>6</v>
+      </c>
+      <c r="F10" s="6">
+        <v>5</v>
+      </c>
+      <c r="G10" s="6">
+        <v>4</v>
+      </c>
+      <c r="H10" s="6">
+        <v>3</v>
+      </c>
+      <c r="I10" s="6">
+        <v>2</v>
+      </c>
+      <c r="J10" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" ht="20" customHeight="1">
+      <c r="A11" t="s" s="3">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s" s="4">
+        <v>36</v>
+      </c>
+      <c r="C11" t="s" s="5">
+        <v>37</v>
+      </c>
+      <c r="D11" s="5">
+        <v>35</v>
+      </c>
+      <c r="E11" s="6">
+        <v>6</v>
+      </c>
+      <c r="F11" s="6">
+        <v>5</v>
+      </c>
+      <c r="G11" s="6">
+        <v>4</v>
+      </c>
+      <c r="H11" s="6">
+        <v>3</v>
+      </c>
+      <c r="I11" s="6">
+        <v>2</v>
+      </c>
+      <c r="J11" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" ht="20" customHeight="1">
+      <c r="A12" t="s" s="3">
+        <v>38</v>
+      </c>
+      <c r="B12" t="s" s="4">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s" s="5">
+        <v>40</v>
+      </c>
+      <c r="D12" s="5">
+        <v>35</v>
+      </c>
+      <c r="E12" s="6">
+        <v>6</v>
+      </c>
+      <c r="F12" s="6">
+        <v>5</v>
+      </c>
+      <c r="G12" s="6">
+        <v>4</v>
+      </c>
+      <c r="H12" s="6">
+        <v>3</v>
+      </c>
+      <c r="I12" s="6">
+        <v>2</v>
+      </c>
+      <c r="J12" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" ht="20" customHeight="1">
+      <c r="A13" t="s" s="3">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s" s="4">
+        <v>42</v>
+      </c>
+      <c r="C13" t="s" s="5">
+        <v>43</v>
+      </c>
+      <c r="D13" s="5">
+        <v>35</v>
+      </c>
+      <c r="E13" s="6">
+        <v>6</v>
+      </c>
+      <c r="F13" s="6">
+        <v>5</v>
+      </c>
+      <c r="G13" s="6">
+        <v>4</v>
+      </c>
+      <c r="H13" s="6">
+        <v>3</v>
+      </c>
+      <c r="I13" s="6">
+        <v>2</v>
+      </c>
+      <c r="J13" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" ht="20" customHeight="1">
+      <c r="A14" t="s" s="3">
+        <v>44</v>
+      </c>
+      <c r="B14" t="s" s="4">
+        <v>45</v>
+      </c>
+      <c r="C14" t="s" s="5">
+        <v>46</v>
+      </c>
+      <c r="D14" s="5">
+        <v>35</v>
+      </c>
+      <c r="E14" s="6">
+        <v>6</v>
+      </c>
+      <c r="F14" s="6">
+        <v>5</v>
+      </c>
+      <c r="G14" s="6">
+        <v>4</v>
+      </c>
+      <c r="H14" s="6">
+        <v>3</v>
+      </c>
+      <c r="I14" s="6">
+        <v>2</v>
+      </c>
+      <c r="J14" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" ht="20" customHeight="1">
+      <c r="A15" t="s" s="3">
+        <v>47</v>
+      </c>
+      <c r="B15" t="s" s="4">
+        <v>48</v>
+      </c>
+      <c r="C15" t="s" s="5">
+        <v>49</v>
+      </c>
+      <c r="D15" s="5">
+        <v>35</v>
+      </c>
+      <c r="E15" s="6">
+        <v>6</v>
+      </c>
+      <c r="F15" s="6">
+        <v>5</v>
+      </c>
+      <c r="G15" s="6">
+        <v>4</v>
+      </c>
+      <c r="H15" s="6">
+        <v>3</v>
+      </c>
+      <c r="I15" s="6">
+        <v>2</v>
+      </c>
+      <c r="J15" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" ht="20" customHeight="1">
+      <c r="A16" t="s" s="3">
+        <v>50</v>
+      </c>
+      <c r="B16" t="s" s="4">
+        <v>51</v>
+      </c>
+      <c r="C16" t="s" s="5">
+        <v>52</v>
+      </c>
+      <c r="D16" s="5">
+        <v>35</v>
+      </c>
+      <c r="E16" s="6">
+        <v>6</v>
+      </c>
+      <c r="F16" s="6">
+        <v>5</v>
+      </c>
+      <c r="G16" s="6">
+        <v>4</v>
+      </c>
+      <c r="H16" s="6">
+        <v>3</v>
+      </c>
+      <c r="I16" s="6">
+        <v>2</v>
+      </c>
+      <c r="J16" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" ht="20" customHeight="1">
+      <c r="A17" t="s" s="3">
+        <v>53</v>
+      </c>
+      <c r="B17" t="s" s="4">
+        <v>54</v>
+      </c>
+      <c r="C17" t="s" s="5">
+        <v>55</v>
+      </c>
+      <c r="D17" s="5">
+        <v>35</v>
+      </c>
+      <c r="E17" s="6">
+        <v>6</v>
+      </c>
+      <c r="F17" s="6">
+        <v>5</v>
+      </c>
+      <c r="G17" s="6">
+        <v>4</v>
+      </c>
+      <c r="H17" s="6">
+        <v>3</v>
+      </c>
+      <c r="I17" s="6">
+        <v>2</v>
+      </c>
+      <c r="J17" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" ht="20" customHeight="1">
+      <c r="A18" t="s" s="3">
+        <v>56</v>
+      </c>
+      <c r="B18" t="s" s="4">
+        <v>57</v>
+      </c>
+      <c r="C18" t="s" s="5">
+        <v>58</v>
+      </c>
+      <c r="D18" s="5">
+        <v>35</v>
+      </c>
+      <c r="E18" s="6">
+        <v>6</v>
+      </c>
+      <c r="F18" s="6">
+        <v>5</v>
+      </c>
+      <c r="G18" s="6">
+        <v>4</v>
+      </c>
+      <c r="H18" s="6">
+        <v>3</v>
+      </c>
+      <c r="I18" s="6">
+        <v>2</v>
+      </c>
+      <c r="J18" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" ht="20" customHeight="1">
+      <c r="A19" t="s" s="3">
+        <v>59</v>
+      </c>
+      <c r="B19" t="s" s="4">
+        <v>60</v>
+      </c>
+      <c r="C19" t="s" s="5">
+        <v>61</v>
+      </c>
+      <c r="D19" s="5">
+        <v>35</v>
+      </c>
+      <c r="E19" s="6">
+        <v>6</v>
+      </c>
+      <c r="F19" s="6">
+        <v>5</v>
+      </c>
+      <c r="G19" s="6">
+        <v>4</v>
+      </c>
+      <c r="H19" s="6">
+        <v>3</v>
+      </c>
+      <c r="I19" s="6">
+        <v>2</v>
+      </c>
+      <c r="J19" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" ht="20" customHeight="1">
+      <c r="A20" t="s" s="3">
+        <v>62</v>
+      </c>
+      <c r="B20" t="s" s="4">
+        <v>63</v>
+      </c>
+      <c r="C20" t="s" s="5">
+        <v>64</v>
+      </c>
+      <c r="D20" s="5">
+        <v>35</v>
+      </c>
+      <c r="E20" s="6">
+        <v>6</v>
+      </c>
+      <c r="F20" s="6">
+        <v>5</v>
+      </c>
+      <c r="G20" s="6">
+        <v>4</v>
+      </c>
+      <c r="H20" s="6">
+        <v>3</v>
+      </c>
+      <c r="I20" s="6">
+        <v>2</v>
+      </c>
+      <c r="J20" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" ht="20" customHeight="1">
+      <c r="A21" t="s" s="3">
+        <v>65</v>
+      </c>
+      <c r="B21" t="s" s="4">
+        <v>66</v>
+      </c>
+      <c r="C21" t="s" s="5">
+        <v>67</v>
+      </c>
+      <c r="D21" s="5">
+        <v>35</v>
+      </c>
+      <c r="E21" s="6">
+        <v>6</v>
+      </c>
+      <c r="F21" s="6">
+        <v>5</v>
+      </c>
+      <c r="G21" s="6">
+        <v>4</v>
+      </c>
+      <c r="H21" s="6">
+        <v>3</v>
+      </c>
+      <c r="I21" s="6">
+        <v>2</v>
+      </c>
+      <c r="J21" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" ht="20" customHeight="1">
+      <c r="A22" t="s" s="3">
+        <v>68</v>
+      </c>
+      <c r="B22" t="s" s="4">
+        <v>69</v>
+      </c>
+      <c r="C22" t="s" s="5">
+        <v>70</v>
+      </c>
+      <c r="D22" s="5">
+        <v>35</v>
+      </c>
+      <c r="E22" s="6">
+        <v>6</v>
+      </c>
+      <c r="F22" s="6">
+        <v>5</v>
+      </c>
+      <c r="G22" s="6">
+        <v>4</v>
+      </c>
+      <c r="H22" s="6">
+        <v>3</v>
+      </c>
+      <c r="I22" s="6">
+        <v>2</v>
+      </c>
+      <c r="J22" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" ht="20" customHeight="1">
+      <c r="A23" t="s" s="3">
+        <v>71</v>
+      </c>
+      <c r="B23" t="s" s="4">
+        <v>72</v>
+      </c>
+      <c r="C23" t="s" s="5">
+        <v>73</v>
+      </c>
+      <c r="D23" s="5">
+        <v>35</v>
+      </c>
+      <c r="E23" s="6">
+        <v>6</v>
+      </c>
+      <c r="F23" s="6">
+        <v>5</v>
+      </c>
+      <c r="G23" s="6">
+        <v>4</v>
+      </c>
+      <c r="H23" s="6">
+        <v>3</v>
+      </c>
+      <c r="I23" s="6">
+        <v>2</v>
+      </c>
+      <c r="J23" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" ht="20" customHeight="1">
+      <c r="A24" t="s" s="3">
+        <v>74</v>
+      </c>
+      <c r="B24" t="s" s="4">
+        <v>75</v>
+      </c>
+      <c r="C24" t="s" s="5">
+        <v>76</v>
+      </c>
+      <c r="D24" s="5">
+        <v>35</v>
+      </c>
+      <c r="E24" s="6">
+        <v>6</v>
+      </c>
+      <c r="F24" s="6">
+        <v>5</v>
+      </c>
+      <c r="G24" s="6">
+        <v>4</v>
+      </c>
+      <c r="H24" s="6">
+        <v>3</v>
+      </c>
+      <c r="I24" s="6">
+        <v>2</v>
+      </c>
+      <c r="J24" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" ht="20" customHeight="1">
+      <c r="A25" t="s" s="3">
+        <v>77</v>
+      </c>
+      <c r="B25" t="s" s="4">
+        <v>78</v>
+      </c>
+      <c r="C25" t="s" s="5">
+        <v>79</v>
+      </c>
+      <c r="D25" s="5">
+        <v>35</v>
+      </c>
+      <c r="E25" s="6">
+        <v>6</v>
+      </c>
+      <c r="F25" s="6">
+        <v>5</v>
+      </c>
+      <c r="G25" s="6">
+        <v>4</v>
+      </c>
+      <c r="H25" s="6">
+        <v>3</v>
+      </c>
+      <c r="I25" s="6">
+        <v>2</v>
+      </c>
+      <c r="J25" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" ht="20" customHeight="1">
+      <c r="A26" t="s" s="3">
+        <v>80</v>
+      </c>
+      <c r="B26" t="s" s="4">
+        <v>81</v>
+      </c>
+      <c r="C26" t="s" s="5">
+        <v>82</v>
+      </c>
+      <c r="D26" s="5">
+        <v>35</v>
+      </c>
+      <c r="E26" s="6">
+        <v>6</v>
+      </c>
+      <c r="F26" s="6">
+        <v>5</v>
+      </c>
+      <c r="G26" s="6">
+        <v>4</v>
+      </c>
+      <c r="H26" s="6">
+        <v>3</v>
+      </c>
+      <c r="I26" s="6">
+        <v>2</v>
+      </c>
+      <c r="J26" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" ht="20" customHeight="1">
+      <c r="A27" t="s" s="3">
+        <v>83</v>
+      </c>
+      <c r="B27" t="s" s="4">
+        <v>84</v>
+      </c>
+      <c r="C27" t="s" s="5">
+        <v>85</v>
+      </c>
+      <c r="D27" s="5">
+        <v>35</v>
+      </c>
+      <c r="E27" s="6">
+        <v>6</v>
+      </c>
+      <c r="F27" s="6">
+        <v>5</v>
+      </c>
+      <c r="G27" s="6">
+        <v>4</v>
+      </c>
+      <c r="H27" s="6">
+        <v>3</v>
+      </c>
+      <c r="I27" s="6">
+        <v>2</v>
+      </c>
+      <c r="J27" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" ht="20" customHeight="1">
+      <c r="A28" t="s" s="3">
+        <v>86</v>
+      </c>
+      <c r="B28" t="s" s="4">
+        <v>15</v>
+      </c>
+      <c r="C28" t="s" s="5">
+        <v>87</v>
+      </c>
+      <c r="D28" s="5">
+        <v>35</v>
+      </c>
+      <c r="E28" s="6">
+        <v>6</v>
+      </c>
+      <c r="F28" s="6">
+        <v>5</v>
+      </c>
+      <c r="G28" s="6">
+        <v>4</v>
+      </c>
+      <c r="H28" s="6">
+        <v>3</v>
+      </c>
+      <c r="I28" s="6">
+        <v>2</v>
+      </c>
+      <c r="J28" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" ht="20" customHeight="1">
+      <c r="A29" t="s" s="3">
+        <v>88</v>
+      </c>
+      <c r="B29" t="s" s="4">
+        <v>89</v>
+      </c>
+      <c r="C29" t="s" s="5">
+        <v>90</v>
+      </c>
+      <c r="D29" s="5">
+        <v>35</v>
+      </c>
+      <c r="E29" s="6">
+        <v>6</v>
+      </c>
+      <c r="F29" s="6">
+        <v>5</v>
+      </c>
+      <c r="G29" s="6">
+        <v>4</v>
+      </c>
+      <c r="H29" s="6">
+        <v>3</v>
+      </c>
+      <c r="I29" s="6">
+        <v>2</v>
+      </c>
+      <c r="J29" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" ht="20" customHeight="1">
+      <c r="A30" t="s" s="3">
+        <v>91</v>
+      </c>
+      <c r="B30" t="s" s="4">
+        <v>92</v>
+      </c>
+      <c r="C30" t="s" s="5">
+        <v>93</v>
+      </c>
+      <c r="D30" s="5">
+        <v>35</v>
+      </c>
+      <c r="E30" s="6">
+        <v>6</v>
+      </c>
+      <c r="F30" s="6">
+        <v>5</v>
+      </c>
+      <c r="G30" s="6">
+        <v>4</v>
+      </c>
+      <c r="H30" s="6">
+        <v>3</v>
+      </c>
+      <c r="I30" s="6">
+        <v>2</v>
+      </c>
+      <c r="J30" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" ht="20" customHeight="1">
+      <c r="A31" t="s" s="3">
+        <v>94</v>
+      </c>
+      <c r="B31" t="s" s="4">
+        <v>95</v>
+      </c>
+      <c r="C31" t="s" s="5">
+        <v>96</v>
+      </c>
+      <c r="D31" s="5">
+        <v>35</v>
+      </c>
+      <c r="E31" s="6">
+        <v>6</v>
+      </c>
+      <c r="F31" s="6">
+        <v>5</v>
+      </c>
+      <c r="G31" s="6">
+        <v>4</v>
+      </c>
+      <c r="H31" s="6">
+        <v>3</v>
+      </c>
+      <c r="I31" s="6">
+        <v>2</v>
+      </c>
+      <c r="J31" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" ht="20" customHeight="1">
+      <c r="A32" t="s" s="3">
+        <v>97</v>
+      </c>
+      <c r="B32" t="s" s="4">
+        <v>98</v>
+      </c>
+      <c r="C32" t="s" s="5">
+        <v>99</v>
+      </c>
+      <c r="D32" s="5">
+        <v>35</v>
+      </c>
+      <c r="E32" s="6">
+        <v>6</v>
+      </c>
+      <c r="F32" s="6">
+        <v>5</v>
+      </c>
+      <c r="G32" s="6">
+        <v>4</v>
+      </c>
+      <c r="H32" s="6">
+        <v>3</v>
+      </c>
+      <c r="I32" s="6">
+        <v>2</v>
+      </c>
+      <c r="J32" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" ht="20" customHeight="1">
+      <c r="A33" t="s" s="3">
+        <v>100</v>
+      </c>
+      <c r="B33" t="s" s="4">
+        <v>101</v>
+      </c>
+      <c r="C33" t="s" s="5">
+        <v>102</v>
+      </c>
+      <c r="D33" s="5">
+        <v>35</v>
+      </c>
+      <c r="E33" s="6">
+        <v>6</v>
+      </c>
+      <c r="F33" s="6">
+        <v>5</v>
+      </c>
+      <c r="G33" s="6">
+        <v>4</v>
+      </c>
+      <c r="H33" s="6">
+        <v>3</v>
+      </c>
+      <c r="I33" s="6">
+        <v>2</v>
+      </c>
+      <c r="J33" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" ht="20" customHeight="1">
+      <c r="A34" t="s" s="3">
+        <v>103</v>
+      </c>
+      <c r="B34" t="s" s="4">
+        <v>104</v>
+      </c>
+      <c r="C34" t="s" s="5">
+        <v>105</v>
+      </c>
+      <c r="D34" s="5">
+        <v>35</v>
+      </c>
+      <c r="E34" s="6">
+        <v>6</v>
+      </c>
+      <c r="F34" s="6">
+        <v>5</v>
+      </c>
+      <c r="G34" s="6">
+        <v>4</v>
+      </c>
+      <c r="H34" s="6">
+        <v>3</v>
+      </c>
+      <c r="I34" s="6">
+        <v>2</v>
+      </c>
+      <c r="J34" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" ht="20" customHeight="1">
+      <c r="A35" t="s" s="3">
+        <v>106</v>
+      </c>
+      <c r="B35" t="s" s="4">
+        <v>107</v>
+      </c>
+      <c r="C35" t="s" s="5">
+        <v>108</v>
+      </c>
+      <c r="D35" s="5">
+        <v>35</v>
+      </c>
+      <c r="E35" s="6">
+        <v>6</v>
+      </c>
+      <c r="F35" s="6">
+        <v>5</v>
+      </c>
+      <c r="G35" s="6">
+        <v>4</v>
+      </c>
+      <c r="H35" s="6">
+        <v>3</v>
+      </c>
+      <c r="I35" s="6">
+        <v>2</v>
+      </c>
+      <c r="J35" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" ht="20" customHeight="1">
+      <c r="A36" t="s" s="3">
+        <v>109</v>
+      </c>
+      <c r="B36" t="s" s="4">
+        <v>110</v>
+      </c>
+      <c r="C36" t="s" s="5">
+        <v>111</v>
+      </c>
+      <c r="D36" s="5">
+        <v>35</v>
+      </c>
+      <c r="E36" s="6">
+        <v>6</v>
+      </c>
+      <c r="F36" s="6">
+        <v>5</v>
+      </c>
+      <c r="G36" s="6">
+        <v>4</v>
+      </c>
+      <c r="H36" s="6">
+        <v>3</v>
+      </c>
+      <c r="I36" s="6">
+        <v>2</v>
+      </c>
+      <c r="J36" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" ht="20" customHeight="1">
+      <c r="A37" t="s" s="3">
+        <v>112</v>
+      </c>
+      <c r="B37" t="s" s="4">
+        <v>113</v>
+      </c>
+      <c r="C37" t="s" s="5">
+        <v>114</v>
+      </c>
+      <c r="D37" s="5">
+        <v>35</v>
+      </c>
+      <c r="E37" s="6">
+        <v>6</v>
+      </c>
+      <c r="F37" s="6">
+        <v>5</v>
+      </c>
+      <c r="G37" s="6">
+        <v>4</v>
+      </c>
+      <c r="H37" s="6">
+        <v>3</v>
+      </c>
+      <c r="I37" s="6">
+        <v>2</v>
+      </c>
+      <c r="J37" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" ht="20" customHeight="1">
+      <c r="A38" t="s" s="3">
+        <v>115</v>
+      </c>
+      <c r="B38" t="s" s="4">
+        <v>116</v>
+      </c>
+      <c r="C38" t="s" s="5">
+        <v>117</v>
+      </c>
+      <c r="D38" s="5">
+        <v>35</v>
+      </c>
+      <c r="E38" s="6">
+        <v>6</v>
+      </c>
+      <c r="F38" s="6">
+        <v>5</v>
+      </c>
+      <c r="G38" s="6">
+        <v>4</v>
+      </c>
+      <c r="H38" s="6">
+        <v>3</v>
+      </c>
+      <c r="I38" s="6">
+        <v>2</v>
+      </c>
+      <c r="J38" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" ht="20" customHeight="1">
+      <c r="A39" t="s" s="3">
+        <v>118</v>
+      </c>
+      <c r="B39" t="s" s="4">
+        <v>119</v>
+      </c>
+      <c r="C39" t="s" s="5">
+        <v>120</v>
+      </c>
+      <c r="D39" s="5">
+        <v>35</v>
+      </c>
+      <c r="E39" s="6">
+        <v>6</v>
+      </c>
+      <c r="F39" s="6">
+        <v>5</v>
+      </c>
+      <c r="G39" s="6">
+        <v>4</v>
+      </c>
+      <c r="H39" s="6">
+        <v>3</v>
+      </c>
+      <c r="I39" s="6">
+        <v>2</v>
+      </c>
+      <c r="J39" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" ht="20" customHeight="1">
+      <c r="A40" t="s" s="3">
+        <v>121</v>
+      </c>
+      <c r="B40" t="s" s="4">
+        <v>122</v>
+      </c>
+      <c r="C40" t="s" s="5">
+        <v>123</v>
+      </c>
+      <c r="D40" s="5">
+        <v>35</v>
+      </c>
+      <c r="E40" s="6">
+        <v>6</v>
+      </c>
+      <c r="F40" s="6">
+        <v>5</v>
+      </c>
+      <c r="G40" s="6">
+        <v>4</v>
+      </c>
+      <c r="H40" s="6">
+        <v>3</v>
+      </c>
+      <c r="I40" s="6">
+        <v>2</v>
+      </c>
+      <c r="J40" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" ht="20" customHeight="1">
+      <c r="A41" t="s" s="3">
+        <v>124</v>
+      </c>
+      <c r="B41" t="s" s="4">
+        <v>125</v>
+      </c>
+      <c r="C41" t="s" s="5">
+        <v>126</v>
+      </c>
+      <c r="D41" s="5">
+        <v>35</v>
+      </c>
+      <c r="E41" s="6">
+        <v>6</v>
+      </c>
+      <c r="F41" s="6">
+        <v>5</v>
+      </c>
+      <c r="G41" s="6">
+        <v>4</v>
+      </c>
+      <c r="H41" s="6">
+        <v>3</v>
+      </c>
+      <c r="I41" s="6">
+        <v>2</v>
+      </c>
+      <c r="J41" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" ht="20" customHeight="1">
+      <c r="A42" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="B42" t="s" s="4">
+        <v>128</v>
+      </c>
+      <c r="C42" t="s" s="5">
+        <v>129</v>
+      </c>
+      <c r="D42" s="5">
+        <v>35</v>
+      </c>
+      <c r="E42" s="6">
+        <v>6</v>
+      </c>
+      <c r="F42" s="6">
+        <v>5</v>
+      </c>
+      <c r="G42" s="6">
+        <v>4</v>
+      </c>
+      <c r="H42" s="6">
+        <v>3</v>
+      </c>
+      <c r="I42" s="6">
+        <v>2</v>
+      </c>
+      <c r="J42" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" ht="20" customHeight="1">
+      <c r="A43" t="s" s="3">
+        <v>130</v>
+      </c>
+      <c r="B43" t="s" s="4">
+        <v>131</v>
+      </c>
+      <c r="C43" t="s" s="5">
+        <v>132</v>
+      </c>
+      <c r="D43" s="5">
+        <v>35</v>
+      </c>
+      <c r="E43" s="6">
+        <v>6</v>
+      </c>
+      <c r="F43" s="6">
+        <v>5</v>
+      </c>
+      <c r="G43" s="6">
+        <v>4</v>
+      </c>
+      <c r="H43" s="6">
+        <v>3</v>
+      </c>
+      <c r="I43" s="6">
+        <v>2</v>
+      </c>
+      <c r="J43" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" ht="20" customHeight="1">
+      <c r="A44" t="s" s="3">
+        <v>133</v>
+      </c>
+      <c r="B44" t="s" s="4">
+        <v>134</v>
+      </c>
+      <c r="C44" t="s" s="5">
+        <v>135</v>
+      </c>
+      <c r="D44" s="5">
+        <v>35</v>
+      </c>
+      <c r="E44" s="6">
+        <v>6</v>
+      </c>
+      <c r="F44" s="6">
+        <v>5</v>
+      </c>
+      <c r="G44" s="6">
+        <v>4</v>
+      </c>
+      <c r="H44" s="6">
+        <v>3</v>
+      </c>
+      <c r="I44" s="6">
+        <v>2</v>
+      </c>
+      <c r="J44" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" ht="20" customHeight="1">
+      <c r="A45" t="s" s="3">
+        <v>136</v>
+      </c>
+      <c r="B45" t="s" s="4">
+        <v>137</v>
+      </c>
+      <c r="C45" t="s" s="5">
+        <v>138</v>
+      </c>
+      <c r="D45" s="5">
+        <v>35</v>
+      </c>
+      <c r="E45" s="6">
+        <v>6</v>
+      </c>
+      <c r="F45" s="6">
+        <v>5</v>
+      </c>
+      <c r="G45" s="6">
+        <v>4</v>
+      </c>
+      <c r="H45" s="6">
+        <v>3</v>
+      </c>
+      <c r="I45" s="6">
+        <v>2</v>
+      </c>
+      <c r="J45" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" ht="20" customHeight="1">
+      <c r="A46" t="s" s="3">
+        <v>139</v>
+      </c>
+      <c r="B46" t="s" s="4">
+        <v>140</v>
+      </c>
+      <c r="C46" t="s" s="5">
+        <v>141</v>
+      </c>
+      <c r="D46" s="5">
+        <v>35</v>
+      </c>
+      <c r="E46" s="6">
+        <v>6</v>
+      </c>
+      <c r="F46" s="6">
+        <v>5</v>
+      </c>
+      <c r="G46" s="6">
+        <v>4</v>
+      </c>
+      <c r="H46" s="6">
+        <v>3</v>
+      </c>
+      <c r="I46" s="6">
+        <v>2</v>
+      </c>
+      <c r="J46" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" ht="20" customHeight="1">
+      <c r="A47" t="s" s="3">
+        <v>142</v>
+      </c>
+      <c r="B47" t="s" s="4">
+        <v>143</v>
+      </c>
+      <c r="C47" t="s" s="5">
+        <v>144</v>
+      </c>
+      <c r="D47" s="5">
+        <v>35</v>
+      </c>
+      <c r="E47" s="6">
+        <v>6</v>
+      </c>
+      <c r="F47" s="6">
+        <v>5</v>
+      </c>
+      <c r="G47" s="6">
+        <v>4</v>
+      </c>
+      <c r="H47" s="6">
+        <v>3</v>
+      </c>
+      <c r="I47" s="6">
+        <v>2</v>
+      </c>
+      <c r="J47" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" ht="20" customHeight="1">
+      <c r="A48" t="s" s="3">
+        <v>145</v>
+      </c>
+      <c r="B48" t="s" s="4">
+        <v>146</v>
+      </c>
+      <c r="C48" t="s" s="5">
+        <v>147</v>
+      </c>
+      <c r="D48" s="5">
+        <v>35</v>
+      </c>
+      <c r="E48" s="6">
+        <v>6</v>
+      </c>
+      <c r="F48" s="6">
+        <v>5</v>
+      </c>
+      <c r="G48" s="6">
+        <v>4</v>
+      </c>
+      <c r="H48" s="6">
+        <v>3</v>
+      </c>
+      <c r="I48" s="6">
+        <v>2</v>
+      </c>
+      <c r="J48" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" ht="20" customHeight="1">
+      <c r="A49" t="s" s="3">
+        <v>148</v>
+      </c>
+      <c r="B49" t="s" s="4">
+        <v>149</v>
+      </c>
+      <c r="C49" t="s" s="5">
+        <v>150</v>
+      </c>
+      <c r="D49" s="5">
+        <v>35</v>
+      </c>
+      <c r="E49" s="6">
+        <v>6</v>
+      </c>
+      <c r="F49" s="6">
+        <v>5</v>
+      </c>
+      <c r="G49" s="6">
+        <v>4</v>
+      </c>
+      <c r="H49" s="6">
+        <v>3</v>
+      </c>
+      <c r="I49" s="6">
+        <v>2</v>
+      </c>
+      <c r="J49" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" ht="20" customHeight="1">
+      <c r="A50" t="s" s="3">
+        <v>151</v>
+      </c>
+      <c r="B50" t="s" s="4">
+        <v>152</v>
+      </c>
+      <c r="C50" t="s" s="5">
+        <v>153</v>
+      </c>
+      <c r="D50" s="5">
+        <v>35</v>
+      </c>
+      <c r="E50" s="6">
+        <v>6</v>
+      </c>
+      <c r="F50" s="6">
+        <v>5</v>
+      </c>
+      <c r="G50" s="6">
+        <v>4</v>
+      </c>
+      <c r="H50" s="6">
+        <v>3</v>
+      </c>
+      <c r="I50" s="6">
+        <v>2</v>
+      </c>
+      <c r="J50" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" ht="20" customHeight="1">
+      <c r="A51" t="s" s="3">
+        <v>154</v>
+      </c>
+      <c r="B51" t="s" s="4">
+        <v>155</v>
+      </c>
+      <c r="C51" t="s" s="5">
+        <v>156</v>
+      </c>
+      <c r="D51" s="5">
+        <v>35</v>
+      </c>
+      <c r="E51" s="6">
+        <v>6</v>
+      </c>
+      <c r="F51" s="6">
+        <v>5</v>
+      </c>
+      <c r="G51" s="6">
+        <v>4</v>
+      </c>
+      <c r="H51" s="6">
+        <v>3</v>
+      </c>
+      <c r="I51" s="6">
+        <v>2</v>
+      </c>
+      <c r="J51" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" ht="20" customHeight="1">
+      <c r="A52" t="s" s="3">
+        <v>157</v>
+      </c>
+      <c r="B52" t="s" s="4">
+        <v>158</v>
+      </c>
+      <c r="C52" t="s" s="5">
+        <v>159</v>
+      </c>
+      <c r="D52" s="5">
+        <v>35</v>
+      </c>
+      <c r="E52" s="6">
+        <v>6</v>
+      </c>
+      <c r="F52" s="6">
+        <v>5</v>
+      </c>
+      <c r="G52" s="6">
+        <v>4</v>
+      </c>
+      <c r="H52" s="6">
+        <v>3</v>
+      </c>
+      <c r="I52" s="6">
+        <v>2</v>
+      </c>
+      <c r="J52" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" ht="20" customHeight="1">
+      <c r="A53" t="s" s="3">
+        <v>160</v>
+      </c>
+      <c r="B53" t="s" s="4">
+        <v>161</v>
+      </c>
+      <c r="C53" t="s" s="5">
+        <v>162</v>
+      </c>
+      <c r="D53" s="5">
+        <v>35</v>
+      </c>
+      <c r="E53" s="6">
+        <v>6</v>
+      </c>
+      <c r="F53" s="6">
+        <v>5</v>
+      </c>
+      <c r="G53" s="6">
+        <v>4</v>
+      </c>
+      <c r="H53" s="6">
+        <v>3</v>
+      </c>
+      <c r="I53" s="6">
+        <v>2</v>
+      </c>
+      <c r="J53" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" ht="20" customHeight="1">
+      <c r="A54" t="s" s="3">
+        <v>163</v>
+      </c>
+      <c r="B54" t="s" s="4">
+        <v>164</v>
+      </c>
+      <c r="C54" t="s" s="5">
+        <v>165</v>
+      </c>
+      <c r="D54" s="5">
+        <v>35</v>
+      </c>
+      <c r="E54" s="6">
+        <v>6</v>
+      </c>
+      <c r="F54" s="6">
+        <v>5</v>
+      </c>
+      <c r="G54" s="6">
+        <v>4</v>
+      </c>
+      <c r="H54" s="6">
+        <v>3</v>
+      </c>
+      <c r="I54" s="6">
+        <v>2</v>
+      </c>
+      <c r="J54" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" ht="20" customHeight="1">
+      <c r="A55" t="s" s="3">
+        <v>166</v>
+      </c>
+      <c r="B55" t="s" s="4">
+        <v>167</v>
+      </c>
+      <c r="C55" t="s" s="5">
+        <v>168</v>
+      </c>
+      <c r="D55" s="5">
+        <v>35</v>
+      </c>
+      <c r="E55" s="6">
+        <v>6</v>
+      </c>
+      <c r="F55" s="6">
+        <v>5</v>
+      </c>
+      <c r="G55" s="6">
+        <v>4</v>
+      </c>
+      <c r="H55" s="6">
+        <v>3</v>
+      </c>
+      <c r="I55" s="6">
+        <v>2</v>
+      </c>
+      <c r="J55" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" ht="20" customHeight="1">
+      <c r="A56" t="s" s="3">
+        <v>169</v>
+      </c>
+      <c r="B56" t="s" s="4">
+        <v>170</v>
+      </c>
+      <c r="C56" t="s" s="5">
+        <v>171</v>
+      </c>
+      <c r="D56" s="5">
+        <v>35</v>
+      </c>
+      <c r="E56" s="6">
+        <v>6</v>
+      </c>
+      <c r="F56" s="6">
+        <v>5</v>
+      </c>
+      <c r="G56" s="6">
+        <v>4</v>
+      </c>
+      <c r="H56" s="6">
+        <v>3</v>
+      </c>
+      <c r="I56" s="6">
+        <v>2</v>
+      </c>
+      <c r="J56" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" ht="20" customHeight="1">
+      <c r="A57" t="s" s="3">
+        <v>172</v>
+      </c>
+      <c r="B57" t="s" s="4">
+        <v>173</v>
+      </c>
+      <c r="C57" t="s" s="5">
+        <v>174</v>
+      </c>
+      <c r="D57" s="5">
+        <v>35</v>
+      </c>
+      <c r="E57" s="6">
+        <v>6</v>
+      </c>
+      <c r="F57" s="6">
+        <v>5</v>
+      </c>
+      <c r="G57" s="6">
+        <v>4</v>
+      </c>
+      <c r="H57" s="6">
+        <v>3</v>
+      </c>
+      <c r="I57" s="6">
+        <v>2</v>
+      </c>
+      <c r="J57" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" ht="20" customHeight="1">
+      <c r="A58" t="s" s="3">
+        <v>175</v>
+      </c>
+      <c r="B58" t="s" s="4">
+        <v>176</v>
+      </c>
+      <c r="C58" t="s" s="5">
+        <v>177</v>
+      </c>
+      <c r="D58" s="5">
+        <v>35</v>
+      </c>
+      <c r="E58" s="6">
+        <v>6</v>
+      </c>
+      <c r="F58" s="6">
+        <v>5</v>
+      </c>
+      <c r="G58" s="6">
+        <v>4</v>
+      </c>
+      <c r="H58" s="6">
+        <v>3</v>
+      </c>
+      <c r="I58" s="6">
+        <v>2</v>
+      </c>
+      <c r="J58" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" ht="20" customHeight="1">
+      <c r="A59" t="s" s="3">
+        <v>178</v>
+      </c>
+      <c r="B59" t="s" s="4">
+        <v>179</v>
+      </c>
+      <c r="C59" t="s" s="5">
+        <v>180</v>
+      </c>
+      <c r="D59" s="5">
+        <v>35</v>
+      </c>
+      <c r="E59" s="6">
+        <v>6</v>
+      </c>
+      <c r="F59" s="6">
+        <v>5</v>
+      </c>
+      <c r="G59" s="6">
+        <v>4</v>
+      </c>
+      <c r="H59" s="6">
+        <v>3</v>
+      </c>
+      <c r="I59" s="6">
+        <v>2</v>
+      </c>
+      <c r="J59" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" ht="20" customHeight="1">
+      <c r="A60" t="s" s="3">
+        <v>181</v>
+      </c>
+      <c r="B60" t="s" s="4">
+        <v>182</v>
+      </c>
+      <c r="C60" t="s" s="5">
+        <v>183</v>
+      </c>
+      <c r="D60" s="5">
+        <v>35</v>
+      </c>
+      <c r="E60" s="6">
+        <v>6</v>
+      </c>
+      <c r="F60" s="6">
+        <v>5</v>
+      </c>
+      <c r="G60" s="6">
+        <v>4</v>
+      </c>
+      <c r="H60" s="6">
+        <v>3</v>
+      </c>
+      <c r="I60" s="6">
+        <v>2</v>
+      </c>
+      <c r="J60" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" ht="20" customHeight="1">
+      <c r="A61" t="s" s="3">
+        <v>184</v>
+      </c>
+      <c r="B61" t="s" s="4">
+        <v>185</v>
+      </c>
+      <c r="C61" t="s" s="5">
+        <v>186</v>
+      </c>
+      <c r="D61" s="5">
+        <v>35</v>
+      </c>
+      <c r="E61" s="6">
+        <v>6</v>
+      </c>
+      <c r="F61" s="6">
+        <v>5</v>
+      </c>
+      <c r="G61" s="6">
+        <v>4</v>
+      </c>
+      <c r="H61" s="6">
+        <v>3</v>
+      </c>
+      <c r="I61" s="6">
+        <v>2</v>
+      </c>
+      <c r="J61" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" ht="20" customHeight="1">
+      <c r="A62" t="s" s="3">
+        <v>187</v>
+      </c>
+      <c r="B62" t="s" s="4">
+        <v>188</v>
+      </c>
+      <c r="C62" t="s" s="5">
+        <v>189</v>
+      </c>
+      <c r="D62" s="5">
+        <v>35</v>
+      </c>
+      <c r="E62" s="6">
+        <v>6</v>
+      </c>
+      <c r="F62" s="6">
+        <v>5</v>
+      </c>
+      <c r="G62" s="6">
+        <v>4</v>
+      </c>
+      <c r="H62" s="6">
+        <v>3</v>
+      </c>
+      <c r="I62" s="6">
+        <v>2</v>
+      </c>
+      <c r="J62" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" ht="20" customHeight="1">
+      <c r="A63" t="s" s="3">
+        <v>190</v>
+      </c>
+      <c r="B63" t="s" s="4">
+        <v>191</v>
+      </c>
+      <c r="C63" t="s" s="5">
+        <v>192</v>
+      </c>
+      <c r="D63" s="5">
+        <v>35</v>
+      </c>
+      <c r="E63" s="6">
+        <v>6</v>
+      </c>
+      <c r="F63" s="6">
+        <v>5</v>
+      </c>
+      <c r="G63" s="6">
+        <v>4</v>
+      </c>
+      <c r="H63" s="6">
+        <v>3</v>
+      </c>
+      <c r="I63" s="6">
+        <v>2</v>
+      </c>
+      <c r="J63" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" ht="20" customHeight="1">
+      <c r="A64" t="s" s="3">
+        <v>193</v>
+      </c>
+      <c r="B64" t="s" s="4">
+        <v>194</v>
+      </c>
+      <c r="C64" t="s" s="5">
+        <v>195</v>
+      </c>
+      <c r="D64" s="5">
+        <v>35</v>
+      </c>
+      <c r="E64" s="6">
+        <v>6</v>
+      </c>
+      <c r="F64" s="6">
+        <v>5</v>
+      </c>
+      <c r="G64" s="6">
+        <v>4</v>
+      </c>
+      <c r="H64" s="6">
+        <v>3</v>
+      </c>
+      <c r="I64" s="6">
+        <v>2</v>
+      </c>
+      <c r="J64" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" ht="20" customHeight="1">
+      <c r="A65" t="s" s="3">
+        <v>196</v>
+      </c>
+      <c r="B65" t="s" s="4">
+        <v>197</v>
+      </c>
+      <c r="C65" t="s" s="5">
+        <v>198</v>
+      </c>
+      <c r="D65" s="5">
+        <v>35</v>
+      </c>
+      <c r="E65" s="6">
+        <v>6</v>
+      </c>
+      <c r="F65" s="6">
+        <v>5</v>
+      </c>
+      <c r="G65" s="6">
+        <v>4</v>
+      </c>
+      <c r="H65" s="6">
+        <v>3</v>
+      </c>
+      <c r="I65" s="6">
+        <v>2</v>
+      </c>
+      <c r="J65" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" ht="20" customHeight="1">
+      <c r="A66" t="s" s="3">
+        <v>199</v>
+      </c>
+      <c r="B66" t="s" s="4">
+        <v>200</v>
+      </c>
+      <c r="C66" t="s" s="5">
+        <v>201</v>
+      </c>
+      <c r="D66" s="5">
+        <v>35</v>
+      </c>
+      <c r="E66" s="6">
+        <v>6</v>
+      </c>
+      <c r="F66" s="6">
+        <v>5</v>
+      </c>
+      <c r="G66" s="6">
+        <v>4</v>
+      </c>
+      <c r="H66" s="6">
+        <v>3</v>
+      </c>
+      <c r="I66" s="6">
+        <v>2</v>
+      </c>
+      <c r="J66" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" ht="20" customHeight="1">
+      <c r="A67" t="s" s="3">
+        <v>202</v>
+      </c>
+      <c r="B67" t="s" s="4">
+        <v>203</v>
+      </c>
+      <c r="C67" t="s" s="5">
+        <v>204</v>
+      </c>
+      <c r="D67" s="5">
+        <v>35</v>
+      </c>
+      <c r="E67" s="6">
+        <v>6</v>
+      </c>
+      <c r="F67" s="6">
+        <v>5</v>
+      </c>
+      <c r="G67" s="6">
+        <v>4</v>
+      </c>
+      <c r="H67" s="6">
+        <v>3</v>
+      </c>
+      <c r="I67" s="6">
+        <v>2</v>
+      </c>
+      <c r="J67" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" ht="20" customHeight="1">
+      <c r="A68" t="s" s="3">
+        <v>205</v>
+      </c>
+      <c r="B68" t="s" s="4">
+        <v>206</v>
+      </c>
+      <c r="C68" t="s" s="5">
+        <v>207</v>
+      </c>
+      <c r="D68" s="5">
+        <v>35</v>
+      </c>
+      <c r="E68" s="6">
+        <v>6</v>
+      </c>
+      <c r="F68" s="6">
+        <v>5</v>
+      </c>
+      <c r="G68" s="6">
+        <v>4</v>
+      </c>
+      <c r="H68" s="6">
+        <v>3</v>
+      </c>
+      <c r="I68" s="6">
+        <v>2</v>
+      </c>
+      <c r="J68" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" ht="20" customHeight="1">
+      <c r="A69" t="s" s="3">
+        <v>208</v>
+      </c>
+      <c r="B69" t="s" s="4">
+        <v>209</v>
+      </c>
+      <c r="C69" t="s" s="5">
+        <v>210</v>
+      </c>
+      <c r="D69" s="5">
+        <v>35</v>
+      </c>
+      <c r="E69" s="6">
+        <v>6</v>
+      </c>
+      <c r="F69" s="6">
+        <v>5</v>
+      </c>
+      <c r="G69" s="6">
+        <v>4</v>
+      </c>
+      <c r="H69" s="6">
+        <v>3</v>
+      </c>
+      <c r="I69" s="6">
+        <v>2</v>
+      </c>
+      <c r="J69" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" ht="20" customHeight="1">
+      <c r="A70" t="s" s="3">
+        <v>211</v>
+      </c>
+      <c r="B70" t="s" s="4">
+        <v>212</v>
+      </c>
+      <c r="C70" t="s" s="5">
+        <v>213</v>
+      </c>
+      <c r="D70" s="5">
+        <v>35</v>
+      </c>
+      <c r="E70" s="6">
+        <v>6</v>
+      </c>
+      <c r="F70" s="6">
+        <v>5</v>
+      </c>
+      <c r="G70" s="6">
+        <v>4</v>
+      </c>
+      <c r="H70" s="6">
+        <v>3</v>
+      </c>
+      <c r="I70" s="6">
+        <v>2</v>
+      </c>
+      <c r="J70" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" ht="20" customHeight="1">
+      <c r="A71" t="s" s="3">
+        <v>214</v>
+      </c>
+      <c r="B71" t="s" s="4">
+        <v>215</v>
+      </c>
+      <c r="C71" t="s" s="5">
+        <v>216</v>
+      </c>
+      <c r="D71" s="5">
+        <v>35</v>
+      </c>
+      <c r="E71" s="6">
+        <v>6</v>
+      </c>
+      <c r="F71" s="6">
+        <v>5</v>
+      </c>
+      <c r="G71" s="6">
+        <v>4</v>
+      </c>
+      <c r="H71" s="6">
+        <v>3</v>
+      </c>
+      <c r="I71" s="6">
+        <v>2</v>
+      </c>
+      <c r="J71" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" ht="20" customHeight="1">
+      <c r="A72" t="s" s="3">
+        <v>217</v>
+      </c>
+      <c r="B72" t="s" s="4">
+        <v>218</v>
+      </c>
+      <c r="C72" t="s" s="5">
+        <v>219</v>
+      </c>
+      <c r="D72" s="5">
+        <v>35</v>
+      </c>
+      <c r="E72" s="6">
+        <v>6</v>
+      </c>
+      <c r="F72" s="6">
+        <v>5</v>
+      </c>
+      <c r="G72" s="6">
+        <v>4</v>
+      </c>
+      <c r="H72" s="6">
+        <v>3</v>
+      </c>
+      <c r="I72" s="6">
+        <v>2</v>
+      </c>
+      <c r="J72" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" ht="20" customHeight="1">
+      <c r="A73" t="s" s="3">
+        <v>220</v>
+      </c>
+      <c r="B73" t="s" s="4">
+        <v>221</v>
+      </c>
+      <c r="C73" t="s" s="5">
+        <v>222</v>
+      </c>
+      <c r="D73" s="5">
+        <v>35</v>
+      </c>
+      <c r="E73" s="6">
+        <v>6</v>
+      </c>
+      <c r="F73" s="6">
+        <v>5</v>
+      </c>
+      <c r="G73" s="6">
+        <v>4</v>
+      </c>
+      <c r="H73" s="6">
+        <v>3</v>
+      </c>
+      <c r="I73" s="6">
+        <v>2</v>
+      </c>
+      <c r="J73" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" ht="20" customHeight="1">
+      <c r="A74" t="s" s="3">
+        <v>223</v>
+      </c>
+      <c r="B74" t="s" s="4">
+        <v>224</v>
+      </c>
+      <c r="C74" t="s" s="5">
+        <v>225</v>
+      </c>
+      <c r="D74" s="5">
+        <v>35</v>
+      </c>
+      <c r="E74" s="6">
+        <v>6</v>
+      </c>
+      <c r="F74" s="6">
+        <v>5</v>
+      </c>
+      <c r="G74" s="6">
+        <v>4</v>
+      </c>
+      <c r="H74" s="6">
+        <v>3</v>
+      </c>
+      <c r="I74" s="6">
+        <v>2</v>
+      </c>
+      <c r="J74" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" ht="20" customHeight="1">
+      <c r="A75" t="s" s="3">
+        <v>226</v>
+      </c>
+      <c r="B75" t="s" s="4">
+        <v>227</v>
+      </c>
+      <c r="C75" t="s" s="5">
+        <v>228</v>
+      </c>
+      <c r="D75" s="5">
+        <v>35</v>
+      </c>
+      <c r="E75" s="6">
+        <v>6</v>
+      </c>
+      <c r="F75" s="6">
+        <v>5</v>
+      </c>
+      <c r="G75" s="6">
+        <v>4</v>
+      </c>
+      <c r="H75" s="6">
+        <v>3</v>
+      </c>
+      <c r="I75" s="6">
+        <v>2</v>
+      </c>
+      <c r="J75" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" ht="20" customHeight="1">
+      <c r="A76" t="s" s="3">
+        <v>229</v>
+      </c>
+      <c r="B76" t="s" s="4">
+        <v>230</v>
+      </c>
+      <c r="C76" t="s" s="5">
+        <v>231</v>
+      </c>
+      <c r="D76" s="5">
+        <v>35</v>
+      </c>
+      <c r="E76" s="6">
+        <v>6</v>
+      </c>
+      <c r="F76" s="6">
+        <v>5</v>
+      </c>
+      <c r="G76" s="6">
+        <v>4</v>
+      </c>
+      <c r="H76" s="6">
+        <v>3</v>
+      </c>
+      <c r="I76" s="6">
+        <v>2</v>
+      </c>
+      <c r="J76" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" ht="20" customHeight="1">
+      <c r="A77" t="s" s="3">
+        <v>232</v>
+      </c>
+      <c r="B77" t="s" s="4">
+        <v>233</v>
+      </c>
+      <c r="C77" t="s" s="5">
+        <v>234</v>
+      </c>
+      <c r="D77" s="5">
+        <v>35</v>
+      </c>
+      <c r="E77" s="6">
+        <v>6</v>
+      </c>
+      <c r="F77" s="6">
+        <v>5</v>
+      </c>
+      <c r="G77" s="6">
+        <v>4</v>
+      </c>
+      <c r="H77" s="6">
+        <v>3</v>
+      </c>
+      <c r="I77" s="6">
+        <v>2</v>
+      </c>
+      <c r="J77" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" ht="20" customHeight="1">
+      <c r="A78" t="s" s="3">
+        <v>235</v>
+      </c>
+      <c r="B78" t="s" s="4">
+        <v>236</v>
+      </c>
+      <c r="C78" t="s" s="5">
+        <v>237</v>
+      </c>
+      <c r="D78" s="5">
+        <v>35</v>
+      </c>
+      <c r="E78" s="6">
+        <v>6</v>
+      </c>
+      <c r="F78" s="6">
+        <v>5</v>
+      </c>
+      <c r="G78" s="6">
+        <v>4</v>
+      </c>
+      <c r="H78" s="6">
+        <v>3</v>
+      </c>
+      <c r="I78" s="6">
+        <v>2</v>
+      </c>
+      <c r="J78" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" ht="20" customHeight="1">
+      <c r="A79" t="s" s="3">
+        <v>238</v>
+      </c>
+      <c r="B79" t="s" s="4">
+        <v>239</v>
+      </c>
+      <c r="C79" t="s" s="5">
+        <v>240</v>
+      </c>
+      <c r="D79" s="5">
+        <v>35</v>
+      </c>
+      <c r="E79" s="6">
+        <v>6</v>
+      </c>
+      <c r="F79" s="6">
+        <v>5</v>
+      </c>
+      <c r="G79" s="6">
+        <v>4</v>
+      </c>
+      <c r="H79" s="6">
+        <v>3</v>
+      </c>
+      <c r="I79" s="6">
+        <v>2</v>
+      </c>
+      <c r="J79" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" ht="20" customHeight="1">
+      <c r="A80" t="s" s="3">
+        <v>241</v>
+      </c>
+      <c r="B80" t="s" s="4">
+        <v>242</v>
+      </c>
+      <c r="C80" t="s" s="5">
+        <v>243</v>
+      </c>
+      <c r="D80" s="5">
+        <v>35</v>
+      </c>
+      <c r="E80" s="6">
+        <v>6</v>
+      </c>
+      <c r="F80" s="6">
+        <v>5</v>
+      </c>
+      <c r="G80" s="6">
+        <v>4</v>
+      </c>
+      <c r="H80" s="6">
+        <v>3</v>
+      </c>
+      <c r="I80" s="6">
+        <v>2</v>
+      </c>
+      <c r="J80" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" ht="20" customHeight="1">
+      <c r="A81" t="s" s="3">
+        <v>244</v>
+      </c>
+      <c r="B81" t="s" s="4">
+        <v>245</v>
+      </c>
+      <c r="C81" t="s" s="5">
+        <v>246</v>
+      </c>
+      <c r="D81" s="5">
+        <v>35</v>
+      </c>
+      <c r="E81" s="6">
+        <v>6</v>
+      </c>
+      <c r="F81" s="6">
+        <v>5</v>
+      </c>
+      <c r="G81" s="6">
+        <v>4</v>
+      </c>
+      <c r="H81" s="6">
+        <v>3</v>
+      </c>
+      <c r="I81" s="6">
+        <v>2</v>
+      </c>
+      <c r="J81" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" ht="20" customHeight="1">
+      <c r="A82" t="s" s="3">
+        <v>247</v>
+      </c>
+      <c r="B82" t="s" s="4">
+        <v>248</v>
+      </c>
+      <c r="C82" t="s" s="5">
+        <v>249</v>
+      </c>
+      <c r="D82" s="5">
+        <v>35</v>
+      </c>
+      <c r="E82" s="6">
+        <v>6</v>
+      </c>
+      <c r="F82" s="6">
+        <v>5</v>
+      </c>
+      <c r="G82" s="6">
+        <v>4</v>
+      </c>
+      <c r="H82" s="6">
+        <v>3</v>
+      </c>
+      <c r="I82" s="6">
+        <v>2</v>
+      </c>
+      <c r="J82" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" ht="20" customHeight="1">
+      <c r="A83" t="s" s="3">
+        <v>250</v>
+      </c>
+      <c r="B83" t="s" s="4">
+        <v>251</v>
+      </c>
+      <c r="C83" t="s" s="5">
+        <v>252</v>
+      </c>
+      <c r="D83" s="5">
+        <v>35</v>
+      </c>
+      <c r="E83" s="6">
+        <v>6</v>
+      </c>
+      <c r="F83" s="6">
+        <v>5</v>
+      </c>
+      <c r="G83" s="6">
+        <v>4</v>
+      </c>
+      <c r="H83" s="6">
+        <v>3</v>
+      </c>
+      <c r="I83" s="6">
+        <v>2</v>
+      </c>
+      <c r="J83" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" ht="20" customHeight="1">
+      <c r="A84" t="s" s="3">
+        <v>253</v>
+      </c>
+      <c r="B84" t="s" s="4">
+        <v>254</v>
+      </c>
+      <c r="C84" t="s" s="5">
+        <v>255</v>
+      </c>
+      <c r="D84" s="5">
+        <v>35</v>
+      </c>
+      <c r="E84" s="6">
+        <v>6</v>
+      </c>
+      <c r="F84" s="6">
+        <v>5</v>
+      </c>
+      <c r="G84" s="6">
+        <v>4</v>
+      </c>
+      <c r="H84" s="6">
+        <v>3</v>
+      </c>
+      <c r="I84" s="6">
+        <v>2</v>
+      </c>
+      <c r="J84" s="6">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed #138 TournRPG-138 敵のパラメータ設定
</commit_message>
<xml_diff>
--- a/docs/enemy.xlsx
+++ b/docs/enemy.xlsx
@@ -1143,7 +1143,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1169,6 +1169,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2536,7 +2539,7 @@
         <v>5</v>
       </c>
       <c r="H3" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I3" s="6">
         <v>3</v>
@@ -2571,10 +2574,10 @@
         <v>6</v>
       </c>
       <c r="H4" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I4" s="6">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J4" s="6">
         <v>2</v>
@@ -2599,24 +2602,12 @@
       <c r="E5" s="5">
         <v>35</v>
       </c>
-      <c r="F5" s="6">
-        <v>6</v>
-      </c>
-      <c r="G5" s="6">
-        <v>5</v>
-      </c>
-      <c r="H5" s="6">
-        <v>4</v>
-      </c>
-      <c r="I5" s="6">
-        <v>3</v>
-      </c>
-      <c r="J5" s="6">
-        <v>2</v>
-      </c>
-      <c r="K5" s="6">
-        <v>1</v>
-      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" t="s" s="3">
@@ -2635,13 +2626,13 @@
         <v>35</v>
       </c>
       <c r="F6" s="6">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G6" s="6">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H6" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I6" s="6">
         <v>3</v>
@@ -5471,11 +5462,9 @@
         <v>2</v>
       </c>
       <c r="B4" t="s" s="4">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s" s="4">
-        <v>12</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="C4" s="9"/>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="6"/>
@@ -5490,9 +5479,7 @@
       <c r="C5" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="D5" t="s" s="4">
-        <v>12</v>
-      </c>
+      <c r="D5" s="9"/>
       <c r="E5" s="8"/>
       <c r="F5" s="6"/>
     </row>
@@ -5501,11 +5488,9 @@
         <v>4</v>
       </c>
       <c r="B6" t="s" s="4">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s" s="4">
-        <v>16</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="C6" s="9"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="6"/>
@@ -5514,29 +5499,17 @@
       <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B7" t="s" s="4">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s" s="4">
-        <v>16</v>
-      </c>
-      <c r="D7" t="s" s="4">
-        <v>16</v>
-      </c>
-      <c r="E7" t="s" s="4">
-        <v>16</v>
-      </c>
-      <c r="F7" t="s" s="4">
-        <v>16</v>
-      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" s="3">
         <v>6</v>
       </c>
-      <c r="B8" t="s" s="4">
-        <v>20</v>
-      </c>
+      <c r="B8" s="9"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>

</xml_diff>

<commit_message>
fixed #145 TournRPG-145 SEを追加する
</commit_message>
<xml_diff>
--- a/docs/enemy.xlsx
+++ b/docs/enemy.xlsx
@@ -2526,7 +2526,7 @@
         <v>3</v>
       </c>
       <c r="G3" s="6">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H3" s="6">
         <v>2</v>
@@ -2558,7 +2558,7 @@
         <v>5</v>
       </c>
       <c r="G4" s="6">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H4" s="6">
         <v>3</v>

</xml_diff>

<commit_message>
fixed #204 TournRPG-204 敵の種類を増やす
</commit_message>
<xml_diff>
--- a/docs/enemy.xlsx
+++ b/docs/enemy.xlsx
@@ -51,6 +51,42 @@
     <t>int</t>
   </si>
   <si>
+    <t>SLIME</t>
+  </si>
+  <si>
+    <t>スライム</t>
+  </si>
+  <si>
+    <t>slime</t>
+  </si>
+  <si>
+    <t>e009.png</t>
+  </si>
+  <si>
+    <t>SLIME_2</t>
+  </si>
+  <si>
+    <t>レッドスライム</t>
+  </si>
+  <si>
+    <t>slime_2</t>
+  </si>
+  <si>
+    <t>e009a.png</t>
+  </si>
+  <si>
+    <t>SLIME_3</t>
+  </si>
+  <si>
+    <t>鋼のスライム</t>
+  </si>
+  <si>
+    <t>slime_3</t>
+  </si>
+  <si>
+    <t>e009b.png</t>
+  </si>
+  <si>
     <t>BAT</t>
   </si>
   <si>
@@ -337,42 +373,6 @@
   </si>
   <si>
     <t>e008b.png</t>
-  </si>
-  <si>
-    <t>SLIME</t>
-  </si>
-  <si>
-    <t>スライム</t>
-  </si>
-  <si>
-    <t>slime</t>
-  </si>
-  <si>
-    <t>e009.png</t>
-  </si>
-  <si>
-    <t>SLIME_2</t>
-  </si>
-  <si>
-    <t>レッドスライム</t>
-  </si>
-  <si>
-    <t>slime_2</t>
-  </si>
-  <si>
-    <t>e009a.png</t>
-  </si>
-  <si>
-    <t>SLIME_3</t>
-  </si>
-  <si>
-    <t>鋼のスライム</t>
-  </si>
-  <si>
-    <t>slime_3</t>
-  </si>
-  <si>
-    <t>e009b.png</t>
   </si>
   <si>
     <t>GHOST</t>
@@ -2539,25 +2539,25 @@
         <v>15</v>
       </c>
       <c r="E3" s="5">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F3" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G3" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H3" s="6">
         <v>0</v>
       </c>
       <c r="I3" s="6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J3" s="6">
         <v>0</v>
       </c>
       <c r="K3" s="6">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
@@ -2574,25 +2574,25 @@
         <v>19</v>
       </c>
       <c r="E4" s="5">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F4" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G4" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H4" s="6">
         <v>0</v>
       </c>
       <c r="I4" s="6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J4" s="6">
         <v>0</v>
       </c>
       <c r="K4" s="6">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" ht="20" customHeight="1">
@@ -2609,7 +2609,7 @@
         <v>23</v>
       </c>
       <c r="E5" s="5">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
@@ -2632,16 +2632,16 @@
         <v>27</v>
       </c>
       <c r="E6" s="5">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="F6" s="6">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G6" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H6" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I6" s="6">
         <v>3</v>
@@ -2650,7 +2650,7 @@
         <v>0</v>
       </c>
       <c r="K6" s="6">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" ht="20" customHeight="1">
@@ -2667,7 +2667,7 @@
         <v>31</v>
       </c>
       <c r="E7" s="5">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="F7" s="6">
         <v>6</v>
@@ -2676,16 +2676,16 @@
         <v>5</v>
       </c>
       <c r="H7" s="6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I7" s="6">
         <v>3</v>
       </c>
       <c r="J7" s="6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K7" s="6">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" ht="20" customHeight="1">
@@ -2704,24 +2704,12 @@
       <c r="E8" s="5">
         <v>35</v>
       </c>
-      <c r="F8" s="6">
-        <v>6</v>
-      </c>
-      <c r="G8" s="6">
-        <v>5</v>
-      </c>
-      <c r="H8" s="6">
-        <v>4</v>
-      </c>
-      <c r="I8" s="6">
-        <v>3</v>
-      </c>
-      <c r="J8" s="6">
-        <v>3</v>
-      </c>
-      <c r="K8" s="6">
-        <v>15</v>
-      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" t="s" s="3">
@@ -2737,22 +2725,22 @@
         <v>39</v>
       </c>
       <c r="E9" s="5">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="F9" s="6">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G9" s="6">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H9" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I9" s="6">
         <v>3</v>
       </c>
       <c r="J9" s="6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K9" s="6">
         <v>15</v>
@@ -5482,7 +5470,9 @@
       <c r="B3" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="C3" s="8"/>
+      <c r="C3" t="s" s="5">
+        <v>12</v>
+      </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -5493,7 +5483,7 @@
         <v>1</v>
       </c>
       <c r="I3" s="6">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
@@ -5501,9 +5491,11 @@
         <v>2</v>
       </c>
       <c r="B4" t="s" s="4">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s" s="5">
         <v>16</v>
       </c>
-      <c r="C4" s="9"/>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="6"/>
@@ -5511,10 +5503,10 @@
         <v>1</v>
       </c>
       <c r="H4" s="6">
-        <v>999</v>
+        <v>1</v>
       </c>
       <c r="I4" s="6">
-        <v>3</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" ht="20" customHeight="1">
@@ -5524,20 +5516,22 @@
       <c r="B5" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="C5" t="s" s="4">
+      <c r="C5" t="s" s="5">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="D5" s="9"/>
       <c r="E5" s="8"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6">
         <v>1</v>
       </c>
       <c r="H5" s="6">
-        <v>999</v>
+        <v>1</v>
       </c>
       <c r="I5" s="6">
-        <v>3</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
@@ -5547,7 +5541,9 @@
       <c r="B6" t="s" s="4">
         <v>24</v>
       </c>
-      <c r="C6" s="9"/>
+      <c r="C6" t="s" s="4">
+        <v>12</v>
+      </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="6"/>
@@ -5565,35 +5561,45 @@
       <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
+      <c r="B7" t="s" s="4">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s" s="4">
+        <v>12</v>
+      </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
       <c r="G7" s="6">
-        <v>999</v>
+        <v>2</v>
       </c>
       <c r="H7" s="6">
         <v>999</v>
       </c>
-      <c r="I7" s="9"/>
+      <c r="I7" s="4">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" s="3">
         <v>6</v>
       </c>
-      <c r="B8" s="9"/>
+      <c r="B8" t="s" s="4">
+        <v>36</v>
+      </c>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6">
-        <v>999</v>
+        <v>2</v>
       </c>
       <c r="H8" s="6">
         <v>999</v>
       </c>
-      <c r="I8" s="6"/>
+      <c r="I8" s="6">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fixed #361 TournRPG-361 目潰しを使う敵の作成
</commit_message>
<xml_diff>
--- a/docs/enemy.xlsx
+++ b/docs/enemy.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="345">
   <si>
     <t>id</t>
   </si>
@@ -28,6 +28,9 @@
   </si>
   <si>
     <t>hp</t>
+  </si>
+  <si>
+    <t>mp</t>
   </si>
   <si>
     <t>xp</t>
@@ -2321,7 +2324,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K84"/>
+  <dimension ref="A1:L84"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="C3" xSplit="2" ySplit="2" activePane="bottomRight" state="frozen"/>
@@ -2335,12 +2338,13 @@
     <col min="4" max="4" width="9.85156" style="1" customWidth="1"/>
     <col min="5" max="5" width="6.17188" style="1" customWidth="1"/>
     <col min="6" max="6" width="5.35156" style="1" customWidth="1"/>
-    <col min="7" max="7" width="3.67188" style="1" customWidth="1"/>
-    <col min="8" max="8" width="4.17188" style="1" customWidth="1"/>
-    <col min="9" max="9" width="4" style="1" customWidth="1"/>
-    <col min="10" max="10" width="4.85156" style="1" customWidth="1"/>
-    <col min="11" max="11" width="7" style="1" customWidth="1"/>
-    <col min="12" max="256" width="12" style="1" customWidth="1"/>
+    <col min="7" max="7" width="5.35156" style="1" customWidth="1"/>
+    <col min="8" max="8" width="3.67188" style="1" customWidth="1"/>
+    <col min="9" max="9" width="4.17188" style="1" customWidth="1"/>
+    <col min="10" max="10" width="4" style="1" customWidth="1"/>
+    <col min="11" max="11" width="4.85156" style="1" customWidth="1"/>
+    <col min="12" max="12" width="7" style="1" customWidth="1"/>
+    <col min="13" max="256" width="12" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
@@ -2377,66 +2381,72 @@
       <c r="K1" t="s" s="2">
         <v>10</v>
       </c>
+      <c r="L1" t="s" s="2">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" ht="20" customHeight="1">
       <c r="A2" t="s" s="3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s" s="4">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s" s="4">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s" s="4">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H2" t="s" s="4">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I2" t="s" s="4">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J2" t="s" s="4">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K2" t="s" s="4">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="L2" t="s" s="4">
+        <v>12</v>
       </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" t="s" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s" s="4">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s" s="5">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s" s="5">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E3" s="6">
         <v>10</v>
       </c>
       <c r="F3" s="7">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G3" s="7">
         <v>2</v>
       </c>
       <c r="H3" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I3" s="7">
         <v>0</v>
@@ -2445,33 +2455,36 @@
         <v>0</v>
       </c>
       <c r="K3" s="7">
+        <v>0</v>
+      </c>
+      <c r="L3" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" t="s" s="3">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s" s="4">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s" s="5">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s" s="5">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E4" s="6">
         <v>10</v>
       </c>
       <c r="F4" s="7">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G4" s="7">
         <v>3</v>
       </c>
       <c r="H4" s="7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I4" s="7">
         <v>0</v>
@@ -2480,248 +2493,272 @@
         <v>0</v>
       </c>
       <c r="K4" s="7">
+        <v>0</v>
+      </c>
+      <c r="L4" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" t="s" s="8">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s" s="9">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s" s="10">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s" s="10">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E5" s="11">
         <v>5</v>
       </c>
-      <c r="F5" s="12"/>
+      <c r="F5" s="12">
+        <v>10</v>
+      </c>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" t="s" s="3">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s" s="4">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s" s="5">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s" s="5">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E6" s="6">
         <v>15</v>
       </c>
       <c r="F6" s="7">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G6" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H6" s="7">
+        <v>4</v>
+      </c>
+      <c r="I6" s="7">
         <v>2</v>
       </c>
-      <c r="I6" s="7">
-        <v>3</v>
-      </c>
       <c r="J6" s="7">
+        <v>3</v>
+      </c>
+      <c r="K6" s="7">
         <v>0</v>
       </c>
-      <c r="K6" s="7">
+      <c r="L6" s="7">
         <v>6</v>
       </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" t="s" s="3">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s" s="4">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s" s="5">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s" s="5">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E7" s="6">
         <v>22</v>
       </c>
       <c r="F7" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G7" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H7" s="7">
+        <v>5</v>
+      </c>
+      <c r="I7" s="7">
         <v>1</v>
       </c>
-      <c r="I7" s="7">
-        <v>3</v>
-      </c>
       <c r="J7" s="7">
+        <v>3</v>
+      </c>
+      <c r="K7" s="7">
         <v>0</v>
       </c>
-      <c r="K7" s="7">
+      <c r="L7" s="7">
         <v>4</v>
       </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" t="s" s="3">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s" s="13">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s" s="14">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s" s="14">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E8" s="15">
         <v>35</v>
       </c>
-      <c r="F8" s="16"/>
+      <c r="F8" s="16">
+        <v>10</v>
+      </c>
       <c r="G8" s="16"/>
       <c r="H8" s="16"/>
       <c r="I8" s="16"/>
       <c r="J8" s="16"/>
       <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" t="s" s="3">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s" s="4">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s" s="5">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D9" t="s" s="5">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E9" s="6">
         <v>50</v>
       </c>
       <c r="F9" s="7">
+        <v>10</v>
+      </c>
+      <c r="G9" s="7">
         <v>20</v>
       </c>
-      <c r="G9" s="7">
+      <c r="H9" s="7">
         <v>7</v>
       </c>
-      <c r="H9" s="7">
+      <c r="I9" s="7">
         <v>2</v>
       </c>
-      <c r="I9" s="7">
-        <v>3</v>
-      </c>
       <c r="J9" s="7">
+        <v>3</v>
+      </c>
+      <c r="K9" s="7">
         <v>0</v>
       </c>
-      <c r="K9" s="7">
+      <c r="L9" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" t="s" s="3">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s" s="13">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s" s="14">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s" s="14">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E10" s="15">
         <v>35</v>
       </c>
       <c r="F10" s="16">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G10" s="16">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H10" s="16">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I10" s="16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J10" s="16">
         <v>3</v>
       </c>
       <c r="K10" s="16">
+        <v>3</v>
+      </c>
+      <c r="L10" s="16">
         <v>15</v>
       </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" t="s" s="3">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s" s="13">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s" s="14">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D11" t="s" s="14">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E11" s="15">
         <v>35</v>
       </c>
       <c r="F11" s="16">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G11" s="16">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H11" s="16">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I11" s="16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J11" s="16">
         <v>3</v>
       </c>
       <c r="K11" s="16">
+        <v>3</v>
+      </c>
+      <c r="L11" s="16">
         <v>15</v>
       </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" t="s" s="3">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s" s="4">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s" s="5">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D12" t="s" s="5">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E12" s="6">
         <v>35</v>
       </c>
       <c r="F12" s="7">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G12" s="7">
         <v>5</v>
@@ -2730,2532 +2767,2751 @@
         <v>5</v>
       </c>
       <c r="I12" s="7">
+        <v>5</v>
+      </c>
+      <c r="J12" s="7">
         <v>2</v>
       </c>
-      <c r="J12" s="7">
+      <c r="K12" s="7">
         <v>0</v>
       </c>
-      <c r="K12" s="7">
+      <c r="L12" s="7">
         <v>5</v>
       </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" t="s" s="3">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B13" t="s" s="4">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C13" t="s" s="5">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D13" t="s" s="5">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E13" s="6">
         <v>35</v>
       </c>
       <c r="F13" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G13" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H13" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I13" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J13" s="7">
         <v>3</v>
       </c>
       <c r="K13" s="7">
+        <v>3</v>
+      </c>
+      <c r="L13" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="A14" t="s" s="3">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B14" t="s" s="4">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C14" t="s" s="5">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D14" t="s" s="5">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E14" s="6">
         <v>35</v>
       </c>
       <c r="F14" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G14" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H14" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I14" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J14" s="7">
         <v>3</v>
       </c>
       <c r="K14" s="7">
+        <v>3</v>
+      </c>
+      <c r="L14" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" t="s" s="3">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B15" t="s" s="4">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C15" t="s" s="5">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D15" t="s" s="5">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E15" s="6">
         <v>35</v>
       </c>
       <c r="F15" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G15" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H15" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I15" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J15" s="7">
         <v>3</v>
       </c>
       <c r="K15" s="7">
+        <v>3</v>
+      </c>
+      <c r="L15" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" t="s" s="3">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B16" t="s" s="4">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C16" t="s" s="5">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D16" t="s" s="5">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E16" s="6">
         <v>35</v>
       </c>
       <c r="F16" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G16" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H16" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I16" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J16" s="7">
         <v>3</v>
       </c>
       <c r="K16" s="7">
+        <v>3</v>
+      </c>
+      <c r="L16" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" t="s" s="3">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B17" t="s" s="4">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C17" t="s" s="5">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D17" t="s" s="5">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E17" s="6">
         <v>35</v>
       </c>
       <c r="F17" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G17" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H17" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I17" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J17" s="7">
         <v>3</v>
       </c>
       <c r="K17" s="7">
+        <v>3</v>
+      </c>
+      <c r="L17" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="18" ht="20" customHeight="1">
       <c r="A18" t="s" s="3">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B18" t="s" s="4">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C18" t="s" s="5">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D18" t="s" s="5">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E18" s="6">
         <v>35</v>
       </c>
       <c r="F18" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G18" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H18" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I18" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J18" s="7">
         <v>3</v>
       </c>
       <c r="K18" s="7">
+        <v>3</v>
+      </c>
+      <c r="L18" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" t="s" s="3">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B19" t="s" s="4">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C19" t="s" s="5">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D19" t="s" s="5">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E19" s="6">
         <v>35</v>
       </c>
       <c r="F19" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G19" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H19" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I19" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J19" s="7">
         <v>3</v>
       </c>
       <c r="K19" s="7">
+        <v>3</v>
+      </c>
+      <c r="L19" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" t="s" s="3">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B20" t="s" s="4">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C20" t="s" s="5">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D20" t="s" s="5">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E20" s="6">
         <v>35</v>
       </c>
       <c r="F20" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G20" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H20" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I20" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J20" s="7">
         <v>3</v>
       </c>
       <c r="K20" s="7">
+        <v>3</v>
+      </c>
+      <c r="L20" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" t="s" s="3">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B21" t="s" s="4">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C21" t="s" s="5">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D21" t="s" s="5">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E21" s="6">
         <v>35</v>
       </c>
       <c r="F21" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G21" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H21" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I21" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J21" s="7">
         <v>3</v>
       </c>
       <c r="K21" s="7">
+        <v>3</v>
+      </c>
+      <c r="L21" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" t="s" s="3">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B22" t="s" s="4">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C22" t="s" s="5">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D22" t="s" s="5">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E22" s="6">
         <v>35</v>
       </c>
       <c r="F22" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G22" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H22" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I22" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J22" s="7">
         <v>3</v>
       </c>
       <c r="K22" s="7">
+        <v>3</v>
+      </c>
+      <c r="L22" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" t="s" s="3">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B23" t="s" s="4">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C23" t="s" s="5">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D23" t="s" s="5">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E23" s="6">
         <v>35</v>
       </c>
       <c r="F23" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G23" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H23" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I23" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J23" s="7">
         <v>3</v>
       </c>
       <c r="K23" s="7">
+        <v>3</v>
+      </c>
+      <c r="L23" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" t="s" s="3">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B24" t="s" s="4">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C24" t="s" s="5">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D24" t="s" s="5">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E24" s="6">
         <v>35</v>
       </c>
       <c r="F24" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G24" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H24" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I24" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J24" s="7">
         <v>3</v>
       </c>
       <c r="K24" s="7">
+        <v>3</v>
+      </c>
+      <c r="L24" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" t="s" s="3">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B25" t="s" s="4">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C25" t="s" s="5">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D25" t="s" s="5">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E25" s="6">
         <v>35</v>
       </c>
       <c r="F25" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G25" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H25" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I25" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J25" s="7">
         <v>3</v>
       </c>
       <c r="K25" s="7">
+        <v>3</v>
+      </c>
+      <c r="L25" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" t="s" s="3">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B26" t="s" s="4">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C26" t="s" s="5">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D26" t="s" s="5">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E26" s="6">
         <v>35</v>
       </c>
       <c r="F26" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G26" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H26" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I26" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J26" s="7">
         <v>3</v>
       </c>
       <c r="K26" s="7">
+        <v>3</v>
+      </c>
+      <c r="L26" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" t="s" s="3">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B27" t="s" s="4">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C27" t="s" s="5">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D27" t="s" s="5">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E27" s="6">
         <v>35</v>
       </c>
       <c r="F27" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G27" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H27" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I27" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J27" s="7">
         <v>3</v>
       </c>
       <c r="K27" s="7">
+        <v>3</v>
+      </c>
+      <c r="L27" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="28" ht="20" customHeight="1">
       <c r="A28" t="s" s="3">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B28" t="s" s="4">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C28" t="s" s="5">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D28" t="s" s="5">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E28" s="6">
         <v>35</v>
       </c>
       <c r="F28" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G28" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H28" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I28" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J28" s="7">
         <v>3</v>
       </c>
       <c r="K28" s="7">
+        <v>3</v>
+      </c>
+      <c r="L28" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" t="s" s="3">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B29" t="s" s="4">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C29" t="s" s="5">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D29" t="s" s="5">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E29" s="6">
         <v>35</v>
       </c>
       <c r="F29" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G29" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H29" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I29" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J29" s="7">
         <v>3</v>
       </c>
       <c r="K29" s="7">
+        <v>3</v>
+      </c>
+      <c r="L29" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="30" ht="20" customHeight="1">
       <c r="A30" t="s" s="3">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B30" t="s" s="4">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C30" t="s" s="5">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D30" t="s" s="5">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E30" s="6">
         <v>35</v>
       </c>
       <c r="F30" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G30" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H30" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I30" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J30" s="7">
         <v>3</v>
       </c>
       <c r="K30" s="7">
+        <v>3</v>
+      </c>
+      <c r="L30" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" t="s" s="3">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B31" t="s" s="4">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C31" t="s" s="5">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D31" t="s" s="5">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E31" s="6">
         <v>35</v>
       </c>
       <c r="F31" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G31" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H31" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I31" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J31" s="7">
         <v>3</v>
       </c>
       <c r="K31" s="7">
+        <v>3</v>
+      </c>
+      <c r="L31" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" t="s" s="3">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B32" t="s" s="4">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C32" t="s" s="5">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D32" t="s" s="5">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E32" s="6">
         <v>35</v>
       </c>
       <c r="F32" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G32" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H32" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I32" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J32" s="7">
         <v>3</v>
       </c>
       <c r="K32" s="7">
+        <v>3</v>
+      </c>
+      <c r="L32" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" t="s" s="3">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B33" t="s" s="4">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C33" t="s" s="5">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D33" t="s" s="5">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E33" s="6">
         <v>35</v>
       </c>
       <c r="F33" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G33" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H33" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I33" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J33" s="7">
         <v>3</v>
       </c>
       <c r="K33" s="7">
+        <v>3</v>
+      </c>
+      <c r="L33" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="A34" t="s" s="3">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B34" t="s" s="4">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C34" t="s" s="5">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D34" t="s" s="5">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E34" s="6">
         <v>35</v>
       </c>
       <c r="F34" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G34" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H34" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I34" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J34" s="7">
         <v>3</v>
       </c>
       <c r="K34" s="7">
+        <v>3</v>
+      </c>
+      <c r="L34" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" t="s" s="3">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B35" t="s" s="4">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C35" t="s" s="5">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D35" t="s" s="5">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E35" s="6">
         <v>35</v>
       </c>
       <c r="F35" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G35" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H35" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I35" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J35" s="7">
         <v>3</v>
       </c>
       <c r="K35" s="7">
+        <v>3</v>
+      </c>
+      <c r="L35" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" t="s" s="3">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B36" t="s" s="4">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C36" t="s" s="5">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D36" t="s" s="5">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E36" s="6">
         <v>35</v>
       </c>
       <c r="F36" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G36" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H36" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I36" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J36" s="7">
         <v>3</v>
       </c>
       <c r="K36" s="7">
+        <v>3</v>
+      </c>
+      <c r="L36" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" t="s" s="3">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B37" t="s" s="4">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C37" t="s" s="5">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D37" t="s" s="5">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E37" s="6">
         <v>35</v>
       </c>
       <c r="F37" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G37" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H37" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I37" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J37" s="7">
         <v>3</v>
       </c>
       <c r="K37" s="7">
+        <v>3</v>
+      </c>
+      <c r="L37" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" t="s" s="3">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B38" t="s" s="4">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C38" t="s" s="5">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D38" t="s" s="5">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E38" s="6">
         <v>35</v>
       </c>
       <c r="F38" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G38" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H38" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I38" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J38" s="7">
         <v>3</v>
       </c>
       <c r="K38" s="7">
+        <v>3</v>
+      </c>
+      <c r="L38" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" t="s" s="3">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B39" t="s" s="4">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C39" t="s" s="5">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D39" t="s" s="5">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E39" s="6">
         <v>35</v>
       </c>
       <c r="F39" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G39" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H39" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I39" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J39" s="7">
         <v>3</v>
       </c>
       <c r="K39" s="7">
+        <v>3</v>
+      </c>
+      <c r="L39" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" t="s" s="3">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B40" t="s" s="4">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C40" t="s" s="5">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D40" t="s" s="5">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E40" s="6">
         <v>35</v>
       </c>
       <c r="F40" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G40" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H40" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I40" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J40" s="7">
         <v>3</v>
       </c>
       <c r="K40" s="7">
+        <v>3</v>
+      </c>
+      <c r="L40" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" t="s" s="3">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B41" t="s" s="4">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C41" t="s" s="5">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D41" t="s" s="5">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E41" s="6">
         <v>35</v>
       </c>
       <c r="F41" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G41" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H41" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I41" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J41" s="7">
         <v>3</v>
       </c>
       <c r="K41" s="7">
+        <v>3</v>
+      </c>
+      <c r="L41" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="42" ht="20" customHeight="1">
       <c r="A42" t="s" s="3">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B42" t="s" s="4">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C42" t="s" s="5">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D42" t="s" s="5">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E42" s="6">
         <v>35</v>
       </c>
       <c r="F42" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G42" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H42" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I42" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J42" s="7">
         <v>3</v>
       </c>
       <c r="K42" s="7">
+        <v>3</v>
+      </c>
+      <c r="L42" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" t="s" s="3">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B43" t="s" s="4">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C43" t="s" s="5">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D43" t="s" s="5">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E43" s="6">
         <v>35</v>
       </c>
       <c r="F43" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G43" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H43" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I43" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J43" s="7">
         <v>3</v>
       </c>
       <c r="K43" s="7">
+        <v>3</v>
+      </c>
+      <c r="L43" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" t="s" s="3">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B44" t="s" s="4">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C44" t="s" s="5">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D44" t="s" s="5">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E44" s="6">
         <v>35</v>
       </c>
       <c r="F44" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G44" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H44" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I44" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J44" s="7">
         <v>3</v>
       </c>
       <c r="K44" s="7">
+        <v>3</v>
+      </c>
+      <c r="L44" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" t="s" s="3">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B45" t="s" s="4">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C45" t="s" s="5">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D45" t="s" s="5">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E45" s="6">
         <v>35</v>
       </c>
       <c r="F45" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G45" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H45" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I45" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J45" s="7">
         <v>3</v>
       </c>
       <c r="K45" s="7">
+        <v>3</v>
+      </c>
+      <c r="L45" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" t="s" s="3">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B46" t="s" s="4">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C46" t="s" s="5">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D46" t="s" s="5">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E46" s="6">
         <v>35</v>
       </c>
       <c r="F46" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G46" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H46" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I46" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J46" s="7">
         <v>3</v>
       </c>
       <c r="K46" s="7">
+        <v>3</v>
+      </c>
+      <c r="L46" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" t="s" s="3">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B47" t="s" s="4">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C47" t="s" s="5">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D47" t="s" s="5">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E47" s="6">
         <v>35</v>
       </c>
       <c r="F47" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G47" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H47" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I47" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J47" s="7">
         <v>3</v>
       </c>
       <c r="K47" s="7">
+        <v>3</v>
+      </c>
+      <c r="L47" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" t="s" s="3">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B48" t="s" s="4">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C48" t="s" s="5">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D48" t="s" s="5">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E48" s="6">
         <v>35</v>
       </c>
       <c r="F48" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G48" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H48" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I48" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J48" s="7">
         <v>3</v>
       </c>
       <c r="K48" s="7">
+        <v>3</v>
+      </c>
+      <c r="L48" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" t="s" s="3">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B49" t="s" s="4">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C49" t="s" s="5">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D49" t="s" s="5">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E49" s="6">
         <v>35</v>
       </c>
       <c r="F49" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G49" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H49" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I49" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J49" s="7">
         <v>3</v>
       </c>
       <c r="K49" s="7">
+        <v>3</v>
+      </c>
+      <c r="L49" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" t="s" s="3">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B50" t="s" s="4">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C50" t="s" s="5">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D50" t="s" s="5">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E50" s="6">
         <v>35</v>
       </c>
       <c r="F50" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G50" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H50" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I50" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J50" s="7">
         <v>3</v>
       </c>
       <c r="K50" s="7">
+        <v>3</v>
+      </c>
+      <c r="L50" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" t="s" s="3">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B51" t="s" s="4">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C51" t="s" s="5">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D51" t="s" s="5">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E51" s="6">
         <v>35</v>
       </c>
       <c r="F51" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G51" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H51" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I51" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J51" s="7">
         <v>3</v>
       </c>
       <c r="K51" s="7">
+        <v>3</v>
+      </c>
+      <c r="L51" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" t="s" s="3">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B52" t="s" s="4">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C52" t="s" s="5">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D52" t="s" s="5">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E52" s="6">
         <v>35</v>
       </c>
       <c r="F52" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G52" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H52" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I52" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J52" s="7">
         <v>3</v>
       </c>
       <c r="K52" s="7">
+        <v>3</v>
+      </c>
+      <c r="L52" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" t="s" s="3">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B53" t="s" s="4">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C53" t="s" s="5">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D53" t="s" s="5">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E53" s="6">
         <v>35</v>
       </c>
       <c r="F53" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G53" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H53" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I53" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J53" s="7">
         <v>3</v>
       </c>
       <c r="K53" s="7">
+        <v>3</v>
+      </c>
+      <c r="L53" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="54" ht="20" customHeight="1">
       <c r="A54" t="s" s="3">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B54" t="s" s="4">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C54" t="s" s="5">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D54" t="s" s="5">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E54" s="6">
         <v>35</v>
       </c>
       <c r="F54" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G54" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H54" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I54" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J54" s="7">
         <v>3</v>
       </c>
       <c r="K54" s="7">
+        <v>3</v>
+      </c>
+      <c r="L54" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="55" ht="20" customHeight="1">
       <c r="A55" t="s" s="3">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B55" t="s" s="4">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C55" t="s" s="5">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D55" t="s" s="5">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E55" s="6">
         <v>35</v>
       </c>
       <c r="F55" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G55" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H55" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I55" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J55" s="7">
         <v>3</v>
       </c>
       <c r="K55" s="7">
+        <v>3</v>
+      </c>
+      <c r="L55" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="56" ht="20" customHeight="1">
       <c r="A56" t="s" s="3">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B56" t="s" s="4">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C56" t="s" s="5">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D56" t="s" s="5">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E56" s="6">
         <v>35</v>
       </c>
       <c r="F56" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G56" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H56" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I56" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J56" s="7">
         <v>3</v>
       </c>
       <c r="K56" s="7">
+        <v>3</v>
+      </c>
+      <c r="L56" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="57" ht="20" customHeight="1">
       <c r="A57" t="s" s="3">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B57" t="s" s="4">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C57" t="s" s="5">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D57" t="s" s="5">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="E57" s="6">
         <v>35</v>
       </c>
       <c r="F57" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G57" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H57" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I57" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J57" s="7">
         <v>3</v>
       </c>
       <c r="K57" s="7">
+        <v>3</v>
+      </c>
+      <c r="L57" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="58" ht="20" customHeight="1">
       <c r="A58" t="s" s="3">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B58" t="s" s="4">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C58" t="s" s="5">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D58" t="s" s="5">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E58" s="6">
         <v>35</v>
       </c>
       <c r="F58" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G58" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H58" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I58" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J58" s="7">
         <v>3</v>
       </c>
       <c r="K58" s="7">
+        <v>3</v>
+      </c>
+      <c r="L58" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="59" ht="20" customHeight="1">
       <c r="A59" t="s" s="3">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B59" t="s" s="4">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C59" t="s" s="5">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D59" t="s" s="5">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E59" s="6">
         <v>35</v>
       </c>
       <c r="F59" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G59" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H59" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I59" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J59" s="7">
         <v>3</v>
       </c>
       <c r="K59" s="7">
+        <v>3</v>
+      </c>
+      <c r="L59" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="60" ht="20" customHeight="1">
       <c r="A60" t="s" s="3">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B60" t="s" s="4">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C60" t="s" s="5">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D60" t="s" s="5">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E60" s="6">
         <v>35</v>
       </c>
       <c r="F60" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G60" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H60" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I60" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J60" s="7">
         <v>3</v>
       </c>
       <c r="K60" s="7">
+        <v>3</v>
+      </c>
+      <c r="L60" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="61" ht="20" customHeight="1">
       <c r="A61" t="s" s="3">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B61" t="s" s="4">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C61" t="s" s="5">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D61" t="s" s="5">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E61" s="6">
         <v>35</v>
       </c>
       <c r="F61" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G61" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H61" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I61" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J61" s="7">
         <v>3</v>
       </c>
       <c r="K61" s="7">
+        <v>3</v>
+      </c>
+      <c r="L61" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="62" ht="20" customHeight="1">
       <c r="A62" t="s" s="3">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B62" t="s" s="4">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C62" t="s" s="5">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D62" t="s" s="5">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E62" s="6">
         <v>35</v>
       </c>
       <c r="F62" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G62" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H62" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I62" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J62" s="7">
         <v>3</v>
       </c>
       <c r="K62" s="7">
+        <v>3</v>
+      </c>
+      <c r="L62" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="63" ht="20" customHeight="1">
       <c r="A63" t="s" s="3">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B63" t="s" s="4">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C63" t="s" s="5">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D63" t="s" s="5">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E63" s="6">
         <v>35</v>
       </c>
       <c r="F63" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G63" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H63" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I63" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J63" s="7">
         <v>3</v>
       </c>
       <c r="K63" s="7">
+        <v>3</v>
+      </c>
+      <c r="L63" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="64" ht="20" customHeight="1">
       <c r="A64" t="s" s="3">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B64" t="s" s="4">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C64" t="s" s="5">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D64" t="s" s="5">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E64" s="6">
         <v>35</v>
       </c>
       <c r="F64" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G64" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H64" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I64" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J64" s="7">
         <v>3</v>
       </c>
       <c r="K64" s="7">
+        <v>3</v>
+      </c>
+      <c r="L64" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="65" ht="20" customHeight="1">
       <c r="A65" t="s" s="3">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B65" t="s" s="4">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C65" t="s" s="5">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D65" t="s" s="5">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E65" s="6">
         <v>35</v>
       </c>
       <c r="F65" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G65" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H65" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I65" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J65" s="7">
         <v>3</v>
       </c>
       <c r="K65" s="7">
+        <v>3</v>
+      </c>
+      <c r="L65" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="66" ht="20" customHeight="1">
       <c r="A66" t="s" s="3">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B66" t="s" s="4">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C66" t="s" s="5">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D66" t="s" s="5">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E66" s="6">
         <v>35</v>
       </c>
       <c r="F66" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G66" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H66" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I66" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J66" s="7">
         <v>3</v>
       </c>
       <c r="K66" s="7">
+        <v>3</v>
+      </c>
+      <c r="L66" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="67" ht="20" customHeight="1">
       <c r="A67" t="s" s="3">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B67" t="s" s="4">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C67" t="s" s="5">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D67" t="s" s="5">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="E67" s="6">
         <v>35</v>
       </c>
       <c r="F67" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G67" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H67" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I67" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J67" s="7">
         <v>3</v>
       </c>
       <c r="K67" s="7">
+        <v>3</v>
+      </c>
+      <c r="L67" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="68" ht="20" customHeight="1">
       <c r="A68" t="s" s="3">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B68" t="s" s="4">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C68" t="s" s="5">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D68" t="s" s="5">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="E68" s="6">
         <v>35</v>
       </c>
       <c r="F68" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G68" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H68" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I68" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J68" s="7">
         <v>3</v>
       </c>
       <c r="K68" s="7">
+        <v>3</v>
+      </c>
+      <c r="L68" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="69" ht="20" customHeight="1">
       <c r="A69" t="s" s="3">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B69" t="s" s="4">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C69" t="s" s="5">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D69" t="s" s="5">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E69" s="6">
         <v>35</v>
       </c>
       <c r="F69" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G69" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H69" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I69" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J69" s="7">
         <v>3</v>
       </c>
       <c r="K69" s="7">
+        <v>3</v>
+      </c>
+      <c r="L69" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="70" ht="20" customHeight="1">
       <c r="A70" t="s" s="3">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B70" t="s" s="4">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C70" t="s" s="5">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D70" t="s" s="5">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="E70" s="6">
         <v>35</v>
       </c>
       <c r="F70" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G70" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H70" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I70" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J70" s="7">
         <v>3</v>
       </c>
       <c r="K70" s="7">
+        <v>3</v>
+      </c>
+      <c r="L70" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="71" ht="20" customHeight="1">
       <c r="A71" t="s" s="3">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B71" t="s" s="4">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C71" t="s" s="5">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D71" t="s" s="5">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E71" s="6">
         <v>35</v>
       </c>
       <c r="F71" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G71" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H71" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I71" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J71" s="7">
         <v>3</v>
       </c>
       <c r="K71" s="7">
+        <v>3</v>
+      </c>
+      <c r="L71" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="72" ht="20" customHeight="1">
       <c r="A72" t="s" s="3">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B72" t="s" s="4">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C72" t="s" s="5">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D72" t="s" s="5">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="E72" s="6">
         <v>35</v>
       </c>
       <c r="F72" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G72" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H72" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I72" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J72" s="7">
         <v>3</v>
       </c>
       <c r="K72" s="7">
+        <v>3</v>
+      </c>
+      <c r="L72" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="73" ht="20" customHeight="1">
       <c r="A73" t="s" s="3">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B73" t="s" s="4">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C73" t="s" s="5">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D73" t="s" s="5">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="E73" s="6">
         <v>35</v>
       </c>
       <c r="F73" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G73" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H73" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I73" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J73" s="7">
         <v>3</v>
       </c>
       <c r="K73" s="7">
+        <v>3</v>
+      </c>
+      <c r="L73" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="74" ht="20" customHeight="1">
       <c r="A74" t="s" s="3">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B74" t="s" s="4">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C74" t="s" s="5">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D74" t="s" s="5">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="E74" s="6">
         <v>35</v>
       </c>
       <c r="F74" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G74" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H74" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I74" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J74" s="7">
         <v>3</v>
       </c>
       <c r="K74" s="7">
+        <v>3</v>
+      </c>
+      <c r="L74" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="75" ht="20" customHeight="1">
       <c r="A75" t="s" s="3">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B75" t="s" s="4">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C75" t="s" s="5">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D75" t="s" s="5">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E75" s="6">
         <v>35</v>
       </c>
       <c r="F75" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G75" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H75" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I75" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J75" s="7">
         <v>3</v>
       </c>
       <c r="K75" s="7">
+        <v>3</v>
+      </c>
+      <c r="L75" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="76" ht="20" customHeight="1">
       <c r="A76" t="s" s="3">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B76" t="s" s="4">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C76" t="s" s="5">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D76" t="s" s="5">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="E76" s="6">
         <v>35</v>
       </c>
       <c r="F76" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G76" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H76" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I76" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J76" s="7">
         <v>3</v>
       </c>
       <c r="K76" s="7">
+        <v>3</v>
+      </c>
+      <c r="L76" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="77" ht="20" customHeight="1">
       <c r="A77" t="s" s="3">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B77" t="s" s="4">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C77" t="s" s="5">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D77" t="s" s="5">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="E77" s="6">
         <v>35</v>
       </c>
       <c r="F77" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G77" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H77" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I77" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J77" s="7">
         <v>3</v>
       </c>
       <c r="K77" s="7">
+        <v>3</v>
+      </c>
+      <c r="L77" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="78" ht="20" customHeight="1">
       <c r="A78" t="s" s="3">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B78" t="s" s="4">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C78" t="s" s="5">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D78" t="s" s="5">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E78" s="6">
         <v>35</v>
       </c>
       <c r="F78" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G78" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H78" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I78" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J78" s="7">
         <v>3</v>
       </c>
       <c r="K78" s="7">
+        <v>3</v>
+      </c>
+      <c r="L78" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="79" ht="20" customHeight="1">
       <c r="A79" t="s" s="3">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B79" t="s" s="4">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C79" t="s" s="5">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D79" t="s" s="5">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="E79" s="6">
         <v>35</v>
       </c>
       <c r="F79" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G79" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H79" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I79" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J79" s="7">
         <v>3</v>
       </c>
       <c r="K79" s="7">
+        <v>3</v>
+      </c>
+      <c r="L79" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="80" ht="20" customHeight="1">
       <c r="A80" t="s" s="3">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B80" t="s" s="4">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C80" t="s" s="5">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D80" t="s" s="5">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="E80" s="6">
         <v>35</v>
       </c>
       <c r="F80" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G80" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H80" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I80" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J80" s="7">
         <v>3</v>
       </c>
       <c r="K80" s="7">
+        <v>3</v>
+      </c>
+      <c r="L80" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="81" ht="20" customHeight="1">
       <c r="A81" t="s" s="3">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B81" t="s" s="4">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C81" t="s" s="5">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="D81" t="s" s="5">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="E81" s="6">
         <v>35</v>
       </c>
       <c r="F81" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G81" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H81" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I81" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J81" s="7">
         <v>3</v>
       </c>
       <c r="K81" s="7">
+        <v>3</v>
+      </c>
+      <c r="L81" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="82" ht="20" customHeight="1">
       <c r="A82" t="s" s="3">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B82" t="s" s="4">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C82" t="s" s="5">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D82" t="s" s="5">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="E82" s="6">
         <v>35</v>
       </c>
       <c r="F82" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G82" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H82" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I82" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J82" s="7">
         <v>3</v>
       </c>
       <c r="K82" s="7">
+        <v>3</v>
+      </c>
+      <c r="L82" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="83" ht="20" customHeight="1">
       <c r="A83" t="s" s="3">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B83" t="s" s="4">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C83" t="s" s="5">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D83" t="s" s="5">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="E83" s="6">
         <v>35</v>
       </c>
       <c r="F83" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G83" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H83" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I83" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J83" s="7">
         <v>3</v>
       </c>
       <c r="K83" s="7">
+        <v>3</v>
+      </c>
+      <c r="L83" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="84" ht="20" customHeight="1">
       <c r="A84" t="s" s="3">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B84" t="s" s="4">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C84" t="s" s="5">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D84" t="s" s="5">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="E84" s="6">
         <v>35</v>
       </c>
       <c r="F84" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G84" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H84" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I84" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J84" s="7">
         <v>3</v>
       </c>
       <c r="K84" s="7">
+        <v>3</v>
+      </c>
+      <c r="L84" s="7">
         <v>15</v>
       </c>
     </row>
@@ -5298,57 +5554,57 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D1" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="F1" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="G1" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="H1" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="I1" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="2" ht="20" customHeight="1">
       <c r="A2" t="s" s="3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s" s="4">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s" s="4">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s" s="4">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H2" t="s" s="4">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I2" t="s" s="4">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" ht="20" customHeight="1">
@@ -5356,10 +5612,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s" s="5">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="19"/>
@@ -5379,10 +5635,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s" s="5">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="19"/>
@@ -5402,13 +5658,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s" s="5">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E5" s="19"/>
       <c r="F5" s="7"/>
@@ -5427,10 +5683,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s" s="4">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D6" s="19"/>
       <c r="E6" s="19"/>
@@ -5450,10 +5706,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s" s="4">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D7" s="20"/>
       <c r="E7" s="20"/>
@@ -5473,7 +5729,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s" s="4">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C8" s="19"/>
       <c r="D8" s="19"/>
@@ -5494,10 +5750,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s" s="4">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s" s="5">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="19"/>

</xml_diff>